<commit_message>
First launching time main function
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\Desktop\ASD_Project\"/>
     </mc:Choice>
@@ -28,11 +28,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -378,14 +379,1126 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:C102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1089687.0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>263264.0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>318211.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>40068.0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>11389.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>69496.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>94160.0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>15532.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>43006.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>147840.0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>23823.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>35521.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>290848.0</v>
+      </c>
+      <c r="B6" t="n">
+        <v>17340.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>22249.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>441219.0</v>
+      </c>
+      <c r="B7" t="n">
+        <v>7919.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>19340.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>156608.0</v>
+      </c>
+      <c r="B8" t="n">
+        <v>21143.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>27870.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>29740.0</v>
+      </c>
+      <c r="B9" t="n">
+        <v>14192.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>52530.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>55619.0</v>
+      </c>
+      <c r="B10" t="n">
+        <v>30427.0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>37276.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>126597.0</v>
+      </c>
+      <c r="B11" t="n">
+        <v>8085.0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>29789.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>73856.0</v>
+      </c>
+      <c r="B12" t="n">
+        <v>8611.0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>27903.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>146066.0</v>
+      </c>
+      <c r="B13" t="n">
+        <v>8309.0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>35389.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>408729.0</v>
+      </c>
+      <c r="B14" t="n">
+        <v>6041.0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>21082.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>2685748.0</v>
+      </c>
+      <c r="B15" t="n">
+        <v>3935.0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>14884.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>68071.0</v>
+      </c>
+      <c r="B16" t="n">
+        <v>5488.0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>25358.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>93471.0</v>
+      </c>
+      <c r="B17" t="n">
+        <v>4248.0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>26105.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>99428.0</v>
+      </c>
+      <c r="B18" t="n">
+        <v>5515.0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>26475.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>151570.0</v>
+      </c>
+      <c r="B19" t="n">
+        <v>4023.0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>58755.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>199226.0</v>
+      </c>
+      <c r="B20" t="n">
+        <v>3215.0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>222723.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>140650.0</v>
+      </c>
+      <c r="B21" t="n">
+        <v>844.0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>13127.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>86961.0</v>
+      </c>
+      <c r="B22" t="n">
+        <v>4941.0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>21728.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>23554.0</v>
+      </c>
+      <c r="B23" t="n">
+        <v>10167.0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>25801.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>29315.0</v>
+      </c>
+      <c r="B24" t="n">
+        <v>5562.0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>28075.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>18424.0</v>
+      </c>
+      <c r="B25" t="n">
+        <v>4198.0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>26964.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>125117.0</v>
+      </c>
+      <c r="B26" t="n">
+        <v>4325.0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>14050.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>86529.0</v>
+      </c>
+      <c r="B27" t="n">
+        <v>5224.0</v>
+      </c>
+      <c r="C27" t="n">
+        <v>26417.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>48899.0</v>
+      </c>
+      <c r="B28" t="n">
+        <v>3144.0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>29357.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>68890.0</v>
+      </c>
+      <c r="B29" t="n">
+        <v>2556.0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>22700.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>92182.0</v>
+      </c>
+      <c r="B30" t="n">
+        <v>2296.0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>26498.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>133116.0</v>
+      </c>
+      <c r="B31" t="n">
+        <v>1309.0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>14181.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>1061690.0</v>
+      </c>
+      <c r="B32" t="n">
+        <v>95662.0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>20295.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>50890.0</v>
+      </c>
+      <c r="B33" t="n">
+        <v>2835.0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>28459.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>104597.0</v>
+      </c>
+      <c r="B34" t="n">
+        <v>2366.0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>3034377.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>133519.0</v>
+      </c>
+      <c r="B35" t="n">
+        <v>611.0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>8623.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>97384.0</v>
+      </c>
+      <c r="B36" t="n">
+        <v>1656.0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>12201.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>56322.0</v>
+      </c>
+      <c r="B37" t="n">
+        <v>2209.0</v>
+      </c>
+      <c r="C37" t="n">
+        <v>16086.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>442667.0</v>
+      </c>
+      <c r="B38" t="n">
+        <v>2586.0</v>
+      </c>
+      <c r="C38" t="n">
+        <v>304724.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>129556.0</v>
+      </c>
+      <c r="B39" t="n">
+        <v>1753.0</v>
+      </c>
+      <c r="C39" t="n">
+        <v>5310.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>133310.0</v>
+      </c>
+      <c r="B40" t="n">
+        <v>1350.0</v>
+      </c>
+      <c r="C40" t="n">
+        <v>3835.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>22463.0</v>
+      </c>
+      <c r="B41" t="n">
+        <v>2915.0</v>
+      </c>
+      <c r="C41" t="n">
+        <v>8394.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>118925.0</v>
+      </c>
+      <c r="B42" t="n">
+        <v>860.0</v>
+      </c>
+      <c r="C42" t="n">
+        <v>3412.0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>1131441.0</v>
+      </c>
+      <c r="B43" t="n">
+        <v>1367.0</v>
+      </c>
+      <c r="C43" t="n">
+        <v>5300.0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>104670.0</v>
+      </c>
+      <c r="B44" t="n">
+        <v>282316.0</v>
+      </c>
+      <c r="C44" t="n">
+        <v>6079.0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>62194.0</v>
+      </c>
+      <c r="B45" t="n">
+        <v>2532.0</v>
+      </c>
+      <c r="C45" t="n">
+        <v>8632.0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>69980.0</v>
+      </c>
+      <c r="B46" t="n">
+        <v>1217.0</v>
+      </c>
+      <c r="C46" t="n">
+        <v>4174.0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>19741.0</v>
+      </c>
+      <c r="B47" t="n">
+        <v>3426.0</v>
+      </c>
+      <c r="C47" t="n">
+        <v>10694.0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>129521.0</v>
+      </c>
+      <c r="B48" t="n">
+        <v>382.0</v>
+      </c>
+      <c r="C48" t="n">
+        <v>5288.0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>95954.0</v>
+      </c>
+      <c r="B49" t="n">
+        <v>8824.0</v>
+      </c>
+      <c r="C49" t="n">
+        <v>3820.0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>18010.0</v>
+      </c>
+      <c r="B50" t="n">
+        <v>2585.0</v>
+      </c>
+      <c r="C50" t="n">
+        <v>7660.0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>14311.0</v>
+      </c>
+      <c r="B51" t="n">
+        <v>2623.0</v>
+      </c>
+      <c r="C51" t="n">
+        <v>7870.0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>23244.0</v>
+      </c>
+      <c r="B52" t="n">
+        <v>3062.0</v>
+      </c>
+      <c r="C52" t="n">
+        <v>8153.0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>48035.0</v>
+      </c>
+      <c r="B53" t="n">
+        <v>3217.0</v>
+      </c>
+      <c r="C53" t="n">
+        <v>7826.0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>61647.0</v>
+      </c>
+      <c r="B54" t="n">
+        <v>2298.0</v>
+      </c>
+      <c r="C54" t="n">
+        <v>8250.0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>79360.0</v>
+      </c>
+      <c r="B55" t="n">
+        <v>1469.0</v>
+      </c>
+      <c r="C55" t="n">
+        <v>4110.0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>35519.0</v>
+      </c>
+      <c r="B56" t="n">
+        <v>2451.0</v>
+      </c>
+      <c r="C56" t="n">
+        <v>7682.0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>55099.0</v>
+      </c>
+      <c r="B57" t="n">
+        <v>2236.0</v>
+      </c>
+      <c r="C57" t="n">
+        <v>21473.0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>45258.0</v>
+      </c>
+      <c r="B58" t="n">
+        <v>2642.0</v>
+      </c>
+      <c r="C58" t="n">
+        <v>8685.0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>21468.0</v>
+      </c>
+      <c r="B59" t="n">
+        <v>3132.0</v>
+      </c>
+      <c r="C59" t="n">
+        <v>12071.0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>55722.0</v>
+      </c>
+      <c r="B60" t="n">
+        <v>2155.0</v>
+      </c>
+      <c r="C60" t="n">
+        <v>21678.0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>67150.0</v>
+      </c>
+      <c r="B61" t="n">
+        <v>1702.0</v>
+      </c>
+      <c r="C61" t="n">
+        <v>3631.0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>63725.0</v>
+      </c>
+      <c r="B62" t="n">
+        <v>1790.0</v>
+      </c>
+      <c r="C62" t="n">
+        <v>3557.0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>22209.0</v>
+      </c>
+      <c r="B63" t="n">
+        <v>2369.0</v>
+      </c>
+      <c r="C63" t="n">
+        <v>5539.0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>10759.0</v>
+      </c>
+      <c r="B64" t="n">
+        <v>3064.0</v>
+      </c>
+      <c r="C64" t="n">
+        <v>5445.0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>68157.0</v>
+      </c>
+      <c r="B65" t="n">
+        <v>1557.0</v>
+      </c>
+      <c r="C65" t="n">
+        <v>2907.0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>22002.0</v>
+      </c>
+      <c r="B66" t="n">
+        <v>5366.0</v>
+      </c>
+      <c r="C66" t="n">
+        <v>5745.0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>25866.0</v>
+      </c>
+      <c r="B67" t="n">
+        <v>2418.0</v>
+      </c>
+      <c r="C67" t="n">
+        <v>5278.0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>76331.0</v>
+      </c>
+      <c r="B68" t="n">
+        <v>2346.0</v>
+      </c>
+      <c r="C68" t="n">
+        <v>2652.0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>72770.0</v>
+      </c>
+      <c r="B69" t="n">
+        <v>336.0</v>
+      </c>
+      <c r="C69" t="n">
+        <v>2039.0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>68491.0</v>
+      </c>
+      <c r="B70" t="n">
+        <v>4082.0</v>
+      </c>
+      <c r="C70" t="n">
+        <v>2730.0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>40763.0</v>
+      </c>
+      <c r="B71" t="n">
+        <v>2282.0</v>
+      </c>
+      <c r="C71" t="n">
+        <v>5136.0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>84604.0</v>
+      </c>
+      <c r="B72" t="n">
+        <v>1153.0</v>
+      </c>
+      <c r="C72" t="n">
+        <v>4407.0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>74572.0</v>
+      </c>
+      <c r="B73" t="n">
+        <v>1325.0</v>
+      </c>
+      <c r="C73" t="n">
+        <v>3091.0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>41410.0</v>
+      </c>
+      <c r="B74" t="n">
+        <v>2273.0</v>
+      </c>
+      <c r="C74" t="n">
+        <v>5161.0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>43101.0</v>
+      </c>
+      <c r="B75" t="n">
+        <v>2713.0</v>
+      </c>
+      <c r="C75" t="n">
+        <v>5507.0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>69172.0</v>
+      </c>
+      <c r="B76" t="n">
+        <v>1382.0</v>
+      </c>
+      <c r="C76" t="n">
+        <v>15425.0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>38741.0</v>
+      </c>
+      <c r="B77" t="n">
+        <v>2491.0</v>
+      </c>
+      <c r="C77" t="n">
+        <v>5026.0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>59147.0</v>
+      </c>
+      <c r="B78" t="n">
+        <v>1914.0</v>
+      </c>
+      <c r="C78" t="n">
+        <v>4272.0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>37168.0</v>
+      </c>
+      <c r="B79" t="n">
+        <v>2239.0</v>
+      </c>
+      <c r="C79" t="n">
+        <v>5176.0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>66697.0</v>
+      </c>
+      <c r="B80" t="n">
+        <v>2086.0</v>
+      </c>
+      <c r="C80" t="n">
+        <v>3652.0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>67801.0</v>
+      </c>
+      <c r="B81" t="n">
+        <v>1731.0</v>
+      </c>
+      <c r="C81" t="n">
+        <v>3795.0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>41610.0</v>
+      </c>
+      <c r="B82" t="n">
+        <v>2631.0</v>
+      </c>
+      <c r="C82" t="n">
+        <v>4705.0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>19749.0</v>
+      </c>
+      <c r="B83" t="n">
+        <v>2599.0</v>
+      </c>
+      <c r="C83" t="n">
+        <v>21356.0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>25941.0</v>
+      </c>
+      <c r="B84" t="n">
+        <v>2656.0</v>
+      </c>
+      <c r="C84" t="n">
+        <v>3724.0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>25929.0</v>
+      </c>
+      <c r="B85" t="n">
+        <v>1500.0</v>
+      </c>
+      <c r="C85" t="n">
+        <v>1618.0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>7485.0</v>
+      </c>
+      <c r="B86" t="n">
+        <v>2613.0</v>
+      </c>
+      <c r="C86" t="n">
+        <v>3653.0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>32883.0</v>
+      </c>
+      <c r="B87" t="n">
+        <v>2713.0</v>
+      </c>
+      <c r="C87" t="n">
+        <v>3103.0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>79112.0</v>
+      </c>
+      <c r="B88" t="n">
+        <v>581.0</v>
+      </c>
+      <c r="C88" t="n">
+        <v>1556.0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>49678.0</v>
+      </c>
+      <c r="B89" t="n">
+        <v>2270.0</v>
+      </c>
+      <c r="C89" t="n">
+        <v>3694.0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>58049.0</v>
+      </c>
+      <c r="B90" t="n">
+        <v>2012.0</v>
+      </c>
+      <c r="C90" t="n">
+        <v>2145.0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>29651.0</v>
+      </c>
+      <c r="B91" t="n">
+        <v>2671.0</v>
+      </c>
+      <c r="C91" t="n">
+        <v>3527.0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>3452.0</v>
+      </c>
+      <c r="B92" t="n">
+        <v>2623.0</v>
+      </c>
+      <c r="C92" t="n">
+        <v>3615.0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>42393.0</v>
+      </c>
+      <c r="B93" t="n">
+        <v>2790.0</v>
+      </c>
+      <c r="C93" t="n">
+        <v>3606.0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>44751.0</v>
+      </c>
+      <c r="B94" t="n">
+        <v>2501.0</v>
+      </c>
+      <c r="C94" t="n">
+        <v>76767.0</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>84752.0</v>
+      </c>
+      <c r="B95" t="n">
+        <v>1085.0</v>
+      </c>
+      <c r="C95" t="n">
+        <v>2353.0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>68813.0</v>
+      </c>
+      <c r="B96" t="n">
+        <v>1722.0</v>
+      </c>
+      <c r="C96" t="n">
+        <v>3502.0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>16971.0</v>
+      </c>
+      <c r="B97" t="n">
+        <v>1930.0</v>
+      </c>
+      <c r="C97" t="n">
+        <v>2364.0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>29744.0</v>
+      </c>
+      <c r="B98" t="n">
+        <v>2398.0</v>
+      </c>
+      <c r="C98" t="n">
+        <v>3442.0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>71407.0</v>
+      </c>
+      <c r="B99" t="n">
+        <v>299.0</v>
+      </c>
+      <c r="C99" t="n">
+        <v>1477.0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>68981.0</v>
+      </c>
+      <c r="B100" t="n">
+        <v>1083.0</v>
+      </c>
+      <c r="C100" t="n">
+        <v>1680.0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>65956.0</v>
+      </c>
+      <c r="B101" t="n">
+        <v>1299.0</v>
+      </c>
+      <c r="C101" t="n">
+        <v>1514.0</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>32882.0</v>
+      </c>
+      <c r="B102" t="n">
+        <v>2151.0</v>
+      </c>
+      <c r="C102" t="n">
+        <v>2903.0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Prove di misurazione dei tempi
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\Desktop\ASD_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05340F64-615D-497F-A4D4-68B27A5506A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B272C43D-8019-4C1F-BCC8-838918AFEEBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-18540" yWindow="-996" windowWidth="18648" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,13 +28,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Heap</t>
+  </si>
+  <si>
+    <t>Quick</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Mediane</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -42,16 +55,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -59,12 +86,77 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -379,1126 +471,1161 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:C102"/>
+  <dimension ref="A1:J102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="5"/>
+      <c r="H1">
+        <f>MEDIAN(A2:A102)</f>
+        <v>32200</v>
+      </c>
+      <c r="I1">
+        <f t="shared" ref="I1:J1" si="0">MEDIAN(B2:B102)</f>
+        <v>2150</v>
+      </c>
+      <c r="J1">
+        <f t="shared" si="0"/>
+        <v>5100</v>
+      </c>
+    </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1089687.0</v>
+        <v>695900.0</v>
       </c>
       <c r="B2" t="n">
-        <v>263264.0</v>
+        <v>436900.0</v>
       </c>
       <c r="C2" t="n">
-        <v>318211.0</v>
+        <v>538400.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>40068.0</v>
+        <v>168800.0</v>
       </c>
       <c r="B3" t="n">
-        <v>11389.0</v>
+        <v>10600.0</v>
       </c>
       <c r="C3" t="n">
-        <v>69496.0</v>
+        <v>63700.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>94160.0</v>
+        <v>102600.0</v>
       </c>
       <c r="B4" t="n">
-        <v>15532.0</v>
+        <v>13300.0</v>
       </c>
       <c r="C4" t="n">
-        <v>43006.0</v>
+        <v>25300.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>147840.0</v>
+        <v>173300.0</v>
       </c>
       <c r="B5" t="n">
-        <v>23823.0</v>
+        <v>9933.0</v>
       </c>
       <c r="C5" t="n">
-        <v>35521.0</v>
+        <v>10650.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>290848.0</v>
+        <v>45800.0</v>
       </c>
       <c r="B6" t="n">
-        <v>17340.0</v>
+        <v>13666.0</v>
       </c>
       <c r="C6" t="n">
-        <v>22249.0</v>
+        <v>23100.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>441219.0</v>
+        <v>66000.0</v>
       </c>
       <c r="B7" t="n">
-        <v>7919.0</v>
+        <v>4100.0</v>
       </c>
       <c r="C7" t="n">
-        <v>19340.0</v>
+        <v>36900.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>156608.0</v>
+        <v>15150.0</v>
       </c>
       <c r="B8" t="n">
-        <v>21143.0</v>
+        <v>6900.0</v>
       </c>
       <c r="C8" t="n">
-        <v>27870.0</v>
+        <v>47700.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>29740.0</v>
+        <v>22100.0</v>
       </c>
       <c r="B9" t="n">
-        <v>14192.0</v>
+        <v>11800.0</v>
       </c>
       <c r="C9" t="n">
-        <v>52530.0</v>
+        <v>49600.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>55619.0</v>
+        <v>110200.0</v>
       </c>
       <c r="B10" t="n">
-        <v>30427.0</v>
+        <v>4060.0</v>
       </c>
       <c r="C10" t="n">
-        <v>37276.0</v>
+        <v>10700.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>126597.0</v>
+        <v>84900.0</v>
       </c>
       <c r="B11" t="n">
-        <v>8085.0</v>
+        <v>3883.0</v>
       </c>
       <c r="C11" t="n">
-        <v>29789.0</v>
+        <v>27200.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>73856.0</v>
+        <v>131900.0</v>
       </c>
       <c r="B12" t="n">
-        <v>8611.0</v>
+        <v>6250.0</v>
       </c>
       <c r="C12" t="n">
-        <v>27903.0</v>
+        <v>22200.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>146066.0</v>
+        <v>114900.0</v>
       </c>
       <c r="B13" t="n">
-        <v>8309.0</v>
+        <v>7766.0</v>
       </c>
       <c r="C13" t="n">
-        <v>35389.0</v>
+        <v>8433.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>408729.0</v>
+        <v>89100.0</v>
       </c>
       <c r="B14" t="n">
-        <v>6041.0</v>
+        <v>6900.0</v>
       </c>
       <c r="C14" t="n">
-        <v>21082.0</v>
+        <v>15250.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>2685748.0</v>
+        <v>65200.0</v>
       </c>
       <c r="B15" t="n">
-        <v>3935.0</v>
+        <v>7200.0</v>
       </c>
       <c r="C15" t="n">
-        <v>14884.0</v>
+        <v>24300.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>68071.0</v>
+        <v>9800.0</v>
       </c>
       <c r="B16" t="n">
-        <v>5488.0</v>
+        <v>3728.0</v>
       </c>
       <c r="C16" t="n">
-        <v>25358.0</v>
+        <v>31300.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>93471.0</v>
+        <v>106100.0</v>
       </c>
       <c r="B17" t="n">
-        <v>4248.0</v>
+        <v>2070.0</v>
       </c>
       <c r="C17" t="n">
-        <v>26105.0</v>
+        <v>20100.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>99428.0</v>
+        <v>134200.0</v>
       </c>
       <c r="B18" t="n">
-        <v>5515.0</v>
+        <v>1292.0</v>
       </c>
       <c r="C18" t="n">
-        <v>26475.0</v>
+        <v>22900.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>151570.0</v>
+        <v>70800.0</v>
       </c>
       <c r="B19" t="n">
-        <v>4023.0</v>
+        <v>2150.0</v>
       </c>
       <c r="C19" t="n">
-        <v>58755.0</v>
+        <v>19050.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>199226.0</v>
+        <v>6400.0</v>
       </c>
       <c r="B20" t="n">
-        <v>3215.0</v>
+        <v>10800.0</v>
       </c>
       <c r="C20" t="n">
-        <v>222723.0</v>
+        <v>37300.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>140650.0</v>
+        <v>60200.0</v>
       </c>
       <c r="B21" t="n">
-        <v>844.0</v>
+        <v>2130.0</v>
       </c>
       <c r="C21" t="n">
-        <v>13127.0</v>
+        <v>6900.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>86961.0</v>
+        <v>65700.0</v>
       </c>
       <c r="B22" t="n">
-        <v>4941.0</v>
+        <v>3742.0</v>
       </c>
       <c r="C22" t="n">
-        <v>21728.0</v>
+        <v>12750.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>23554.0</v>
+        <v>727.0</v>
       </c>
       <c r="B23" t="n">
-        <v>10167.0</v>
+        <v>6450.0</v>
       </c>
       <c r="C23" t="n">
-        <v>25801.0</v>
+        <v>30900.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>29315.0</v>
+        <v>88500.0</v>
       </c>
       <c r="B24" t="n">
-        <v>5562.0</v>
+        <v>3444.0</v>
       </c>
       <c r="C24" t="n">
-        <v>28075.0</v>
+        <v>7533.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>18424.0</v>
+        <v>51700.0</v>
       </c>
       <c r="B25" t="n">
-        <v>4198.0</v>
+        <v>703.0</v>
       </c>
       <c r="C25" t="n">
-        <v>26964.0</v>
+        <v>18400.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>125117.0</v>
+        <v>45700.0</v>
       </c>
       <c r="B26" t="n">
-        <v>4325.0</v>
+        <v>6525.0</v>
       </c>
       <c r="C26" t="n">
-        <v>14050.0</v>
+        <v>11250.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>86529.0</v>
+        <v>54600.0</v>
       </c>
       <c r="B27" t="n">
-        <v>5224.0</v>
+        <v>1035.0</v>
       </c>
       <c r="C27" t="n">
-        <v>26417.0</v>
+        <v>6000.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>48899.0</v>
+        <v>94300.0</v>
       </c>
       <c r="B28" t="n">
-        <v>3144.0</v>
+        <v>465.0</v>
       </c>
       <c r="C28" t="n">
-        <v>29357.0</v>
+        <v>4700.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>68890.0</v>
+        <v>43300.0</v>
       </c>
       <c r="B29" t="n">
-        <v>2556.0</v>
+        <v>1393.0</v>
       </c>
       <c r="C29" t="n">
-        <v>22700.0</v>
+        <v>5350.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>92182.0</v>
+        <v>53500.0</v>
       </c>
       <c r="B30" t="n">
-        <v>2296.0</v>
+        <v>1492.0</v>
       </c>
       <c r="C30" t="n">
-        <v>26498.0</v>
+        <v>5350.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>133116.0</v>
+        <v>22700.0</v>
       </c>
       <c r="B31" t="n">
-        <v>1309.0</v>
+        <v>4085.0</v>
       </c>
       <c r="C31" t="n">
-        <v>14181.0</v>
+        <v>3366.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>1061690.0</v>
+        <v>22600.0</v>
       </c>
       <c r="B32" t="n">
-        <v>95662.0</v>
+        <v>1211.0</v>
       </c>
       <c r="C32" t="n">
-        <v>20295.0</v>
+        <v>24800.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>50890.0</v>
+        <v>20400.0</v>
       </c>
       <c r="B33" t="n">
-        <v>2835.0</v>
+        <v>1325.0</v>
       </c>
       <c r="C33" t="n">
-        <v>28459.0</v>
+        <v>4620.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>104597.0</v>
+        <v>32500.0</v>
       </c>
       <c r="B34" t="n">
-        <v>2366.0</v>
+        <v>703.0</v>
       </c>
       <c r="C34" t="n">
-        <v>3034377.0</v>
+        <v>1927.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>133519.0</v>
+        <v>10400.0</v>
       </c>
       <c r="B35" t="n">
-        <v>611.0</v>
+        <v>2750.0</v>
       </c>
       <c r="C35" t="n">
-        <v>8623.0</v>
+        <v>7366.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>97384.0</v>
+        <v>34000.0</v>
       </c>
       <c r="B36" t="n">
-        <v>1656.0</v>
+        <v>545.0</v>
       </c>
       <c r="C36" t="n">
-        <v>12201.0</v>
+        <v>2020.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>56322.0</v>
+        <v>22700.0</v>
       </c>
       <c r="B37" t="n">
-        <v>2209.0</v>
+        <v>1268.0</v>
       </c>
       <c r="C37" t="n">
-        <v>16086.0</v>
+        <v>4100.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>442667.0</v>
+        <v>1716.0</v>
       </c>
       <c r="B38" t="n">
-        <v>2586.0</v>
+        <v>2862.0</v>
       </c>
       <c r="C38" t="n">
-        <v>304724.0</v>
+        <v>7366.0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>129556.0</v>
+        <v>16000.0</v>
       </c>
       <c r="B39" t="n">
-        <v>1753.0</v>
+        <v>2255.0</v>
       </c>
       <c r="C39" t="n">
-        <v>5310.0</v>
+        <v>7966.0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>133310.0</v>
+        <v>16800.0</v>
       </c>
       <c r="B40" t="n">
-        <v>1350.0</v>
+        <v>2577.0</v>
       </c>
       <c r="C40" t="n">
-        <v>3835.0</v>
+        <v>7500.0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>22463.0</v>
+        <v>4340.0</v>
       </c>
       <c r="B41" t="n">
-        <v>2915.0</v>
+        <v>2612.0</v>
       </c>
       <c r="C41" t="n">
-        <v>8394.0</v>
+        <v>7866.0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>118925.0</v>
+        <v>32200.0</v>
       </c>
       <c r="B42" t="n">
-        <v>860.0</v>
+        <v>2080.0</v>
       </c>
       <c r="C42" t="n">
-        <v>3412.0</v>
+        <v>9175.0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>1131441.0</v>
+        <v>32900.0</v>
       </c>
       <c r="B43" t="n">
-        <v>1367.0</v>
+        <v>816.0</v>
       </c>
       <c r="C43" t="n">
-        <v>5300.0</v>
+        <v>3057.0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>104670.0</v>
+        <v>55700.0</v>
       </c>
       <c r="B44" t="n">
-        <v>282316.0</v>
+        <v>1045.0</v>
       </c>
       <c r="C44" t="n">
-        <v>6079.0</v>
+        <v>25700.0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>62194.0</v>
+        <v>57900.0</v>
       </c>
       <c r="B45" t="n">
-        <v>2532.0</v>
+        <v>210.0</v>
       </c>
       <c r="C45" t="n">
-        <v>8632.0</v>
+        <v>2488.0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>69980.0</v>
+        <v>29200.0</v>
       </c>
       <c r="B46" t="n">
-        <v>1217.0</v>
+        <v>1004.0</v>
       </c>
       <c r="C46" t="n">
-        <v>4174.0</v>
+        <v>1890.0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>19741.0</v>
+        <v>38600.0</v>
       </c>
       <c r="B47" t="n">
-        <v>3426.0</v>
+        <v>1936.0</v>
       </c>
       <c r="C47" t="n">
-        <v>10694.0</v>
+        <v>5325.0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>129521.0</v>
+        <v>34800.0</v>
       </c>
       <c r="B48" t="n">
-        <v>382.0</v>
+        <v>824.0</v>
       </c>
       <c r="C48" t="n">
-        <v>5288.0</v>
+        <v>1758.0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>95954.0</v>
+        <v>474.0</v>
       </c>
       <c r="B49" t="n">
-        <v>8824.0</v>
+        <v>1716.0</v>
       </c>
       <c r="C49" t="n">
-        <v>3820.0</v>
+        <v>2525.0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>18010.0</v>
+        <v>27800.0</v>
       </c>
       <c r="B50" t="n">
-        <v>2585.0</v>
+        <v>990.0</v>
       </c>
       <c r="C50" t="n">
-        <v>7660.0</v>
+        <v>1725.0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>14311.0</v>
+        <v>13800.0</v>
       </c>
       <c r="B51" t="n">
-        <v>2623.0</v>
+        <v>2650.0</v>
       </c>
       <c r="C51" t="n">
-        <v>7870.0</v>
+        <v>5150.0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>23244.0</v>
+        <v>2985.0</v>
       </c>
       <c r="B52" t="n">
-        <v>3062.0</v>
+        <v>2355.0</v>
       </c>
       <c r="C52" t="n">
-        <v>8153.0</v>
+        <v>2725.0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>48035.0</v>
+        <v>83100.0</v>
       </c>
       <c r="B53" t="n">
-        <v>3217.0</v>
+        <v>2942.0</v>
       </c>
       <c r="C53" t="n">
-        <v>7826.0</v>
+        <v>11200.0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>61647.0</v>
+        <v>12100.0</v>
       </c>
       <c r="B54" t="n">
-        <v>2298.0</v>
+        <v>1584.0</v>
       </c>
       <c r="C54" t="n">
-        <v>8250.0</v>
+        <v>3042.0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>79360.0</v>
+        <v>20250.0</v>
       </c>
       <c r="B55" t="n">
-        <v>1469.0</v>
+        <v>1393.0</v>
       </c>
       <c r="C55" t="n">
-        <v>4110.0</v>
+        <v>2525.0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>35519.0</v>
+        <v>20300.0</v>
       </c>
       <c r="B56" t="n">
-        <v>2451.0</v>
+        <v>1426.0</v>
       </c>
       <c r="C56" t="n">
-        <v>7682.0</v>
+        <v>2550.0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>55099.0</v>
+        <v>4066.0</v>
       </c>
       <c r="B57" t="n">
-        <v>2236.0</v>
+        <v>1741.0</v>
       </c>
       <c r="C57" t="n">
-        <v>21473.0</v>
+        <v>2837.0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>45258.0</v>
+        <v>35000.0</v>
       </c>
       <c r="B58" t="n">
-        <v>2642.0</v>
+        <v>525.0</v>
       </c>
       <c r="C58" t="n">
-        <v>8685.0</v>
+        <v>1325.0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>21468.0</v>
+        <v>5160.0</v>
       </c>
       <c r="B59" t="n">
-        <v>3132.0</v>
+        <v>1872.0</v>
       </c>
       <c r="C59" t="n">
-        <v>12071.0</v>
+        <v>2550.0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>55722.0</v>
+        <v>50800.0</v>
       </c>
       <c r="B60" t="n">
-        <v>2155.0</v>
+        <v>703.0</v>
       </c>
       <c r="C60" t="n">
-        <v>21678.0</v>
+        <v>1380.0</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>67150.0</v>
+        <v>31100.0</v>
       </c>
       <c r="B61" t="n">
-        <v>1702.0</v>
+        <v>1607.0</v>
       </c>
       <c r="C61" t="n">
-        <v>3631.0</v>
+        <v>2050.0</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>63725.0</v>
+        <v>40400.0</v>
       </c>
       <c r="B62" t="n">
-        <v>1790.0</v>
+        <v>2060.0</v>
       </c>
       <c r="C62" t="n">
-        <v>3557.0</v>
+        <v>9466.0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>22209.0</v>
+        <v>2562.0</v>
       </c>
       <c r="B63" t="n">
-        <v>2369.0</v>
+        <v>2388.0</v>
       </c>
       <c r="C63" t="n">
-        <v>5539.0</v>
+        <v>5325.0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>10759.0</v>
+        <v>62100.0</v>
       </c>
       <c r="B64" t="n">
-        <v>3064.0</v>
+        <v>725.0</v>
       </c>
       <c r="C64" t="n">
-        <v>5445.0</v>
+        <v>2090.0</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>68157.0</v>
+        <v>61800.0</v>
       </c>
       <c r="B65" t="n">
-        <v>1557.0</v>
+        <v>1716.0</v>
       </c>
       <c r="C65" t="n">
-        <v>2907.0</v>
+        <v>2662.0</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>22002.0</v>
+        <v>58000.0</v>
       </c>
       <c r="B66" t="n">
-        <v>5366.0</v>
+        <v>7066.0</v>
       </c>
       <c r="C66" t="n">
-        <v>5745.0</v>
+        <v>5250.0</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>25866.0</v>
+        <v>17900.0</v>
       </c>
       <c r="B67" t="n">
-        <v>2418.0</v>
+        <v>2625.0</v>
       </c>
       <c r="C67" t="n">
-        <v>5278.0</v>
+        <v>3733.0</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>76331.0</v>
+        <v>48100.0</v>
       </c>
       <c r="B68" t="n">
-        <v>2346.0</v>
+        <v>1094.0</v>
       </c>
       <c r="C68" t="n">
-        <v>2652.0</v>
+        <v>2485.0</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>72770.0</v>
+        <v>29000.0</v>
       </c>
       <c r="B69" t="n">
-        <v>336.0</v>
+        <v>1557.0</v>
       </c>
       <c r="C69" t="n">
-        <v>2039.0</v>
+        <v>6800.0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>68491.0</v>
+        <v>6500.0</v>
       </c>
       <c r="B70" t="n">
-        <v>4082.0</v>
+        <v>1646.0</v>
       </c>
       <c r="C70" t="n">
-        <v>2730.0</v>
+        <v>4740.0</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>40763.0</v>
+        <v>40800.0</v>
       </c>
       <c r="B71" t="n">
-        <v>2282.0</v>
+        <v>1927.0</v>
       </c>
       <c r="C71" t="n">
-        <v>5136.0</v>
+        <v>4520.0</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>84604.0</v>
+        <v>58400.0</v>
       </c>
       <c r="B72" t="n">
-        <v>1153.0</v>
+        <v>1229.0</v>
       </c>
       <c r="C72" t="n">
-        <v>4407.0</v>
+        <v>1872.0</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>74572.0</v>
+        <v>58200.0</v>
       </c>
       <c r="B73" t="n">
-        <v>1325.0</v>
+        <v>2700.0</v>
       </c>
       <c r="C73" t="n">
-        <v>3091.0</v>
+        <v>1758.0</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>41410.0</v>
+        <v>168200.0</v>
       </c>
       <c r="B74" t="n">
-        <v>2273.0</v>
+        <v>1775.0</v>
       </c>
       <c r="C74" t="n">
-        <v>5161.0</v>
+        <v>4280.0</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>43101.0</v>
+        <v>36800.0</v>
       </c>
       <c r="B75" t="n">
-        <v>2713.0</v>
+        <v>1945.0</v>
       </c>
       <c r="C75" t="n">
-        <v>5507.0</v>
+        <v>2957.0</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>69172.0</v>
+        <v>51800.0</v>
       </c>
       <c r="B76" t="n">
-        <v>1382.0</v>
+        <v>559.0</v>
       </c>
       <c r="C76" t="n">
-        <v>15425.0</v>
+        <v>1450.0</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>38741.0</v>
+        <v>33300.0</v>
       </c>
       <c r="B77" t="n">
-        <v>2491.0</v>
+        <v>2220.0</v>
       </c>
       <c r="C77" t="n">
-        <v>5026.0</v>
+        <v>3766.0</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>59147.0</v>
+        <v>2762.0</v>
       </c>
       <c r="B78" t="n">
-        <v>1914.0</v>
+        <v>2466.0</v>
       </c>
       <c r="C78" t="n">
-        <v>4272.0</v>
+        <v>3450.0</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>37168.0</v>
+        <v>60900.0</v>
       </c>
       <c r="B79" t="n">
-        <v>2239.0</v>
+        <v>904.0</v>
       </c>
       <c r="C79" t="n">
-        <v>5176.0</v>
+        <v>594.0</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>66697.0</v>
+        <v>36700.0</v>
       </c>
       <c r="B80" t="n">
-        <v>2086.0</v>
+        <v>780.0</v>
       </c>
       <c r="C80" t="n">
-        <v>3652.0</v>
+        <v>908.0</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>67801.0</v>
+        <v>49800.0</v>
       </c>
       <c r="B81" t="n">
-        <v>1731.0</v>
+        <v>2050.0</v>
       </c>
       <c r="C81" t="n">
-        <v>3795.0</v>
+        <v>3566.0</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>41610.0</v>
+        <v>14150.0</v>
       </c>
       <c r="B82" t="n">
-        <v>2631.0</v>
+        <v>2800.0</v>
       </c>
       <c r="C82" t="n">
-        <v>4705.0</v>
+        <v>3414.0</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>19749.0</v>
+        <v>87000.0</v>
       </c>
       <c r="B83" t="n">
-        <v>2599.0</v>
+        <v>7733.0</v>
       </c>
       <c r="C83" t="n">
-        <v>21356.0</v>
+        <v>2355.0</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>25941.0</v>
+        <v>12500.0</v>
       </c>
       <c r="B84" t="n">
-        <v>2656.0</v>
+        <v>2775.0</v>
       </c>
       <c r="C84" t="n">
-        <v>3724.0</v>
+        <v>4440.0</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>25929.0</v>
+        <v>28100.0</v>
       </c>
       <c r="B85" t="n">
-        <v>1500.0</v>
+        <v>654.0</v>
       </c>
       <c r="C85" t="n">
-        <v>1618.0</v>
+        <v>1100.0</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>7485.0</v>
+        <v>28800.0</v>
       </c>
       <c r="B86" t="n">
-        <v>2613.0</v>
+        <v>824.0</v>
       </c>
       <c r="C86" t="n">
-        <v>3653.0</v>
+        <v>7400.0</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>32883.0</v>
+        <v>60500.0</v>
       </c>
       <c r="B87" t="n">
-        <v>2713.0</v>
+        <v>1954.0</v>
       </c>
       <c r="C87" t="n">
-        <v>3103.0</v>
+        <v>2650.0</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>79112.0</v>
+        <v>8433.0</v>
       </c>
       <c r="B88" t="n">
-        <v>581.0</v>
+        <v>2525.0</v>
       </c>
       <c r="C88" t="n">
-        <v>1556.0</v>
+        <v>3583.0</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>49678.0</v>
+        <v>46500.0</v>
       </c>
       <c r="B89" t="n">
-        <v>2270.0</v>
+        <v>2427.0</v>
       </c>
       <c r="C89" t="n">
-        <v>3694.0</v>
+        <v>2255.0</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>58049.0</v>
+        <v>9033.0</v>
       </c>
       <c r="B90" t="n">
-        <v>2012.0</v>
+        <v>1553.0</v>
       </c>
       <c r="C90" t="n">
-        <v>2145.0</v>
+        <v>1854.0</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>29651.0</v>
+        <v>25200.0</v>
       </c>
       <c r="B91" t="n">
-        <v>2671.0</v>
+        <v>3700.0</v>
       </c>
       <c r="C91" t="n">
-        <v>3527.0</v>
+        <v>1262.0</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>3452.0</v>
+        <v>24700.0</v>
       </c>
       <c r="B92" t="n">
-        <v>2623.0</v>
+        <v>904.0</v>
       </c>
       <c r="C92" t="n">
-        <v>3615.0</v>
+        <v>1464.0</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>42393.0</v>
+        <v>10333.0</v>
       </c>
       <c r="B93" t="n">
-        <v>2790.0</v>
+        <v>1669.0</v>
       </c>
       <c r="C93" t="n">
-        <v>3606.0</v>
+        <v>2050.0</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>44751.0</v>
+        <v>548.0</v>
       </c>
       <c r="B94" t="n">
-        <v>2501.0</v>
+        <v>2466.0</v>
       </c>
       <c r="C94" t="n">
-        <v>76767.0</v>
+        <v>3633.0</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>84752.0</v>
+        <v>37700.0</v>
       </c>
       <c r="B95" t="n">
-        <v>1085.0</v>
+        <v>2170.0</v>
       </c>
       <c r="C95" t="n">
-        <v>2353.0</v>
+        <v>3450.0</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>68813.0</v>
+        <v>20600.0</v>
       </c>
       <c r="B96" t="n">
-        <v>1722.0</v>
+        <v>1386.0</v>
       </c>
       <c r="C96" t="n">
-        <v>3502.0</v>
+        <v>1863.0</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>16971.0</v>
+        <v>23100.0</v>
       </c>
       <c r="B97" t="n">
-        <v>1930.0</v>
+        <v>1133.0</v>
       </c>
       <c r="C97" t="n">
-        <v>2364.0</v>
+        <v>1122.0</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>29744.0</v>
+        <v>7200.0</v>
       </c>
       <c r="B98" t="n">
-        <v>2398.0</v>
+        <v>1600.0</v>
       </c>
       <c r="C98" t="n">
-        <v>3442.0</v>
+        <v>1683.0</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>71407.0</v>
+        <v>11700.0</v>
       </c>
       <c r="B99" t="n">
-        <v>299.0</v>
+        <v>2675.0</v>
       </c>
       <c r="C99" t="n">
-        <v>1477.0</v>
+        <v>4460.0</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>68981.0</v>
+        <v>57900.0</v>
       </c>
       <c r="B100" t="n">
-        <v>1083.0</v>
+        <v>465.0</v>
       </c>
       <c r="C100" t="n">
-        <v>1680.0</v>
+        <v>922.0</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>65956.0</v>
+        <v>28300.0</v>
       </c>
       <c r="B101" t="n">
-        <v>1299.0</v>
+        <v>886.0</v>
       </c>
       <c r="C101" t="n">
-        <v>1514.0</v>
+        <v>637.0</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>32882.0</v>
+        <v>41900.0</v>
       </c>
       <c r="B102" t="n">
-        <v>2151.0</v>
+        <v>803.0</v>
       </c>
       <c r="C102" t="n">
-        <v>2903.0</v>
+        <v>882.0</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C103">
+    <sortCondition descending="1" ref="A1"/>
+  </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Doesn't build sometimes, trying to solve the error
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -510,1113 +510,1113 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>3763886.0</v>
+        <v>2835675.0</v>
       </c>
       <c r="B2" t="n">
-        <v>296377.0</v>
+        <v>396830.0</v>
       </c>
       <c r="C2" t="n">
-        <v>513547.0</v>
+        <v>516517.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>607549.0</v>
+        <v>690706.0</v>
       </c>
       <c r="B3" t="n">
-        <v>26358.0</v>
+        <v>31272.0</v>
       </c>
       <c r="C3" t="n">
-        <v>76773.0</v>
+        <v>54819.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>398548.0</v>
+        <v>513873.0</v>
       </c>
       <c r="B4" t="n">
-        <v>21797.0</v>
+        <v>18858.0</v>
       </c>
       <c r="C4" t="n">
-        <v>44312.0</v>
+        <v>70746.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>99918.0</v>
+        <v>62932.0</v>
       </c>
       <c r="B5" t="n">
-        <v>26029.0</v>
+        <v>29557.0</v>
       </c>
       <c r="C5" t="n">
-        <v>38390.0</v>
+        <v>66616.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>260576.0</v>
+        <v>530932.0</v>
       </c>
       <c r="B6" t="n">
-        <v>34921.0</v>
+        <v>12548.0</v>
       </c>
       <c r="C6" t="n">
-        <v>81628.0</v>
+        <v>38633.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>46047.0</v>
+        <v>3368250.0</v>
       </c>
       <c r="B7" t="n">
-        <v>43318.0</v>
+        <v>24746.0</v>
       </c>
       <c r="C7" t="n">
-        <v>54284.0</v>
+        <v>58113.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>36315.0</v>
+        <v>44191.0</v>
       </c>
       <c r="B8" t="n">
-        <v>21364.0</v>
+        <v>35852.0</v>
       </c>
       <c r="C8" t="n">
-        <v>80176.0</v>
+        <v>49424.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>346575.0</v>
+        <v>4024608.0</v>
       </c>
       <c r="B9" t="n">
-        <v>26657.0</v>
+        <v>37692.0</v>
       </c>
       <c r="C9" t="n">
-        <v>38738.0</v>
+        <v>58406.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>88107.0</v>
+        <v>260116.0</v>
       </c>
       <c r="B10" t="n">
-        <v>14056.0</v>
+        <v>15265.0</v>
       </c>
       <c r="C10" t="n">
-        <v>32476.0</v>
+        <v>28442.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>507880.0</v>
+        <v>477943.0</v>
       </c>
       <c r="B11" t="n">
-        <v>17477.0</v>
+        <v>7259.0</v>
       </c>
       <c r="C11" t="n">
-        <v>32017.0</v>
+        <v>24126.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>150164.0</v>
+        <v>1503173.0</v>
       </c>
       <c r="B12" t="n">
-        <v>30400.0</v>
+        <v>9984.0</v>
       </c>
       <c r="C12" t="n">
-        <v>39679.0</v>
+        <v>292995.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>377468.0</v>
+        <v>420217.0</v>
       </c>
       <c r="B13" t="n">
-        <v>38791.0</v>
+        <v>13868.0</v>
       </c>
       <c r="C13" t="n">
-        <v>37360.0</v>
+        <v>31842.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>234236.0</v>
+        <v>175397.0</v>
       </c>
       <c r="B14" t="n">
-        <v>22310.0</v>
+        <v>9468.0</v>
       </c>
       <c r="C14" t="n">
-        <v>39866.0</v>
+        <v>37975.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>20699.0</v>
+        <v>44574.0</v>
       </c>
       <c r="B15" t="n">
-        <v>19383.0</v>
+        <v>15145.0</v>
       </c>
       <c r="C15" t="n">
-        <v>40433.0</v>
+        <v>32382.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>212724.0</v>
+        <v>440140.0</v>
       </c>
       <c r="B16" t="n">
-        <v>22739.0</v>
+        <v>9746.0</v>
       </c>
       <c r="C16" t="n">
-        <v>41183.0</v>
+        <v>36070.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>150835.0</v>
+        <v>44162.0</v>
       </c>
       <c r="B17" t="n">
-        <v>41108.0</v>
+        <v>9466.0</v>
       </c>
       <c r="C17" t="n">
-        <v>36898.0</v>
+        <v>38740.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>55875.0</v>
+        <v>52174.0</v>
       </c>
       <c r="B18" t="n">
-        <v>16225.0</v>
+        <v>12546.0</v>
       </c>
       <c r="C18" t="n">
-        <v>33474.0</v>
+        <v>31203.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>399177.0</v>
+        <v>419443.0</v>
       </c>
       <c r="B19" t="n">
-        <v>9129.0</v>
+        <v>13490.0</v>
       </c>
       <c r="C19" t="n">
-        <v>35145.0</v>
+        <v>34802.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>249913.0</v>
+        <v>253996.0</v>
       </c>
       <c r="B20" t="n">
-        <v>14507.0</v>
+        <v>13379.0</v>
       </c>
       <c r="C20" t="n">
-        <v>40511.0</v>
+        <v>32303.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>322674.0</v>
+        <v>402142.0</v>
       </c>
       <c r="B21" t="n">
-        <v>12555.0</v>
+        <v>4687.0</v>
       </c>
       <c r="C21" t="n">
-        <v>37407.0</v>
+        <v>31712.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>357786.0</v>
+        <v>398354.0</v>
       </c>
       <c r="B22" t="n">
-        <v>12670.0</v>
+        <v>7005.0</v>
       </c>
       <c r="C22" t="n">
-        <v>41647.0</v>
+        <v>30731.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>460007.0</v>
+        <v>275852.0</v>
       </c>
       <c r="B23" t="n">
-        <v>7120.0</v>
+        <v>11888.0</v>
       </c>
       <c r="C23" t="n">
-        <v>33807.0</v>
+        <v>41129.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>369713.0</v>
+        <v>340534.0</v>
       </c>
       <c r="B24" t="n">
-        <v>11794.0</v>
+        <v>10792.0</v>
       </c>
       <c r="C24" t="n">
-        <v>30283.0</v>
+        <v>36047.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>608115.0</v>
+        <v>290893.0</v>
       </c>
       <c r="B25" t="n">
-        <v>17160.0</v>
+        <v>10248.0</v>
       </c>
       <c r="C25" t="n">
-        <v>1705498.0</v>
+        <v>38098.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>456428.0</v>
+        <v>2558656.0</v>
       </c>
       <c r="B26" t="n">
-        <v>12040.0</v>
+        <v>10680.0</v>
       </c>
       <c r="C26" t="n">
-        <v>41295.0</v>
+        <v>36637.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>113905.0</v>
+        <v>25327.0</v>
       </c>
       <c r="B27" t="n">
-        <v>8534.0</v>
+        <v>7579.0</v>
       </c>
       <c r="C27" t="n">
-        <v>34548.0</v>
+        <v>44740.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>407847.0</v>
+        <v>221751.0</v>
       </c>
       <c r="B28" t="n">
-        <v>7689.0</v>
+        <v>7268.0</v>
       </c>
       <c r="C28" t="n">
-        <v>35889.0</v>
+        <v>36734.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>403972.0</v>
+        <v>228116.0</v>
       </c>
       <c r="B29" t="n">
-        <v>5176.0</v>
+        <v>5308.0</v>
       </c>
       <c r="C29" t="n">
-        <v>27451.0</v>
+        <v>33062.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>8356.0</v>
+        <v>65024.0</v>
       </c>
       <c r="B30" t="n">
-        <v>6610.0</v>
+        <v>7674.0</v>
       </c>
       <c r="C30" t="n">
-        <v>35756.0</v>
+        <v>43213.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>169834.0</v>
+        <v>128837.0</v>
       </c>
       <c r="B31" t="n">
-        <v>13655.0</v>
+        <v>32051.0</v>
       </c>
       <c r="C31" t="n">
-        <v>41035.0</v>
+        <v>39192.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>184227.0</v>
+        <v>221337.0</v>
       </c>
       <c r="B32" t="n">
-        <v>9200.0</v>
+        <v>7271.0</v>
       </c>
       <c r="C32" t="n">
-        <v>34538.0</v>
+        <v>42157.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>5042.0</v>
+        <v>181460.0</v>
       </c>
       <c r="B33" t="n">
-        <v>7566.0</v>
+        <v>5193.0</v>
       </c>
       <c r="C33" t="n">
-        <v>31689.0</v>
+        <v>22719.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1312.0</v>
+        <v>223208.0</v>
       </c>
       <c r="B34" t="n">
-        <v>7904.0</v>
+        <v>2713.0</v>
       </c>
       <c r="C34" t="n">
-        <v>31884.0</v>
+        <v>24659.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>216637.0</v>
+        <v>217685.0</v>
       </c>
       <c r="B35" t="n">
-        <v>11829.0</v>
+        <v>3330.0</v>
       </c>
       <c r="C35" t="n">
-        <v>37358.0</v>
+        <v>23189.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>340144.0</v>
+        <v>118492.0</v>
       </c>
       <c r="B36" t="n">
-        <v>8430.0</v>
+        <v>5776.0</v>
       </c>
       <c r="C36" t="n">
-        <v>43132.0</v>
+        <v>26158.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>374355.0</v>
+        <v>322886.0</v>
       </c>
       <c r="B37" t="n">
-        <v>7780.0</v>
+        <v>2667.0</v>
       </c>
       <c r="C37" t="n">
-        <v>24390.0</v>
+        <v>16213.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>174618.0</v>
+        <v>51454.0</v>
       </c>
       <c r="B38" t="n">
-        <v>9032.0</v>
+        <v>5667.0</v>
       </c>
       <c r="C38" t="n">
-        <v>25347.0</v>
+        <v>4542177.0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>11282.0</v>
+        <v>17021.0</v>
       </c>
       <c r="B39" t="n">
-        <v>9340.0</v>
+        <v>5800.0</v>
       </c>
       <c r="C39" t="n">
-        <v>52600.0</v>
+        <v>53632.0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>241694.0</v>
+        <v>190833.0</v>
       </c>
       <c r="B40" t="n">
-        <v>10180.0</v>
+        <v>2319.0</v>
       </c>
       <c r="C40" t="n">
-        <v>23271.0</v>
+        <v>37048.0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>244068.0</v>
+        <v>197787.0</v>
       </c>
       <c r="B41" t="n">
-        <v>12313.0</v>
+        <v>2395.0</v>
       </c>
       <c r="C41" t="n">
-        <v>33436.0</v>
+        <v>10931.0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>384859.0</v>
+        <v>172445.0</v>
       </c>
       <c r="B42" t="n">
-        <v>6947.0</v>
+        <v>4036.0</v>
       </c>
       <c r="C42" t="n">
-        <v>11519.0</v>
+        <v>12144.0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>366842.0</v>
+        <v>50222.0</v>
       </c>
       <c r="B43" t="n">
-        <v>7219.0</v>
+        <v>5036.0</v>
       </c>
       <c r="C43" t="n">
-        <v>14617.0</v>
+        <v>12392.0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>420736.0</v>
+        <v>111734.0</v>
       </c>
       <c r="B44" t="n">
-        <v>7848.0</v>
+        <v>5752.0</v>
       </c>
       <c r="C44" t="n">
-        <v>11828.0</v>
+        <v>14556.0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>248069.0</v>
+        <v>32363.0</v>
       </c>
       <c r="B45" t="n">
-        <v>11747.0</v>
+        <v>5456.0</v>
       </c>
       <c r="C45" t="n">
-        <v>13613.0</v>
+        <v>11383.0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>1277.0</v>
+        <v>200967.0</v>
       </c>
       <c r="B46" t="n">
-        <v>7640.0</v>
+        <v>1351.0</v>
       </c>
       <c r="C46" t="n">
-        <v>8803.0</v>
+        <v>11089.0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>349320.0</v>
+        <v>161393.0</v>
       </c>
       <c r="B47" t="n">
-        <v>12588.0</v>
+        <v>4468.0</v>
       </c>
       <c r="C47" t="n">
-        <v>5746.0</v>
+        <v>10652.0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>59358.0</v>
+        <v>264034.0</v>
       </c>
       <c r="B48" t="n">
-        <v>10580.0</v>
+        <v>3332.0</v>
       </c>
       <c r="C48" t="n">
-        <v>10819.0</v>
+        <v>19177.0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>433055.0</v>
+        <v>155328.0</v>
       </c>
       <c r="B49" t="n">
-        <v>843.0</v>
+        <v>4711.0</v>
       </c>
       <c r="C49" t="n">
-        <v>7275.0</v>
+        <v>13599.0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>50394.0</v>
+        <v>166897.0</v>
       </c>
       <c r="B50" t="n">
-        <v>14207.0</v>
+        <v>4363.0</v>
       </c>
       <c r="C50" t="n">
-        <v>11955.0</v>
+        <v>11643.0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>117338.0</v>
+        <v>17980.0</v>
       </c>
       <c r="B51" t="n">
-        <v>11349.0</v>
+        <v>5515.0</v>
       </c>
       <c r="C51" t="n">
-        <v>13865.0</v>
+        <v>11277.0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>237423.0</v>
+        <v>172040.0</v>
       </c>
       <c r="B52" t="n">
-        <v>13288.0</v>
+        <v>1240.0</v>
       </c>
       <c r="C52" t="n">
-        <v>13800.0</v>
+        <v>12485.0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>306217.0</v>
+        <v>121472.0</v>
       </c>
       <c r="B53" t="n">
-        <v>1143082.0</v>
+        <v>4646.0</v>
       </c>
       <c r="C53" t="n">
-        <v>13586.0</v>
+        <v>8099.0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>369287.0</v>
+        <v>85330.0</v>
       </c>
       <c r="B54" t="n">
-        <v>9720.0</v>
+        <v>6612.0</v>
       </c>
       <c r="C54" t="n">
-        <v>12988.0</v>
+        <v>8839.0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>46253.0</v>
+        <v>64292.0</v>
       </c>
       <c r="B55" t="n">
-        <v>15881.0</v>
+        <v>6379.0</v>
       </c>
       <c r="C55" t="n">
-        <v>14523.0</v>
+        <v>9531.0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>166320.0</v>
+        <v>142770.0</v>
       </c>
       <c r="B56" t="n">
-        <v>8290.0</v>
+        <v>5141.0</v>
       </c>
       <c r="C56" t="n">
-        <v>14051.0</v>
+        <v>10108.0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>163793.0</v>
+        <v>43909.0</v>
       </c>
       <c r="B57" t="n">
-        <v>8918.0</v>
+        <v>5917.0</v>
       </c>
       <c r="C57" t="n">
-        <v>14347.0</v>
+        <v>7474.0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>408575.0</v>
+        <v>21183.0</v>
       </c>
       <c r="B58" t="n">
-        <v>3138.0</v>
+        <v>5804.0</v>
       </c>
       <c r="C58" t="n">
-        <v>15273.0</v>
+        <v>6812.0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>396431.0</v>
+        <v>24135.0</v>
       </c>
       <c r="B59" t="n">
-        <v>4177.0</v>
+        <v>4480.0</v>
       </c>
       <c r="C59" t="n">
-        <v>10842.0</v>
+        <v>7909.0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>429977.0</v>
+        <v>98724.0</v>
       </c>
       <c r="B60" t="n">
-        <v>7816.0</v>
+        <v>4315.0</v>
       </c>
       <c r="C60" t="n">
-        <v>12157.0</v>
+        <v>8132.0</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>397894.0</v>
+        <v>187953.0</v>
       </c>
       <c r="B61" t="n">
-        <v>9757.0</v>
+        <v>2316.0</v>
       </c>
       <c r="C61" t="n">
-        <v>12506.0</v>
+        <v>7182.0</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>315621.0</v>
+        <v>51959.0</v>
       </c>
       <c r="B62" t="n">
-        <v>9573.0</v>
+        <v>4870.0</v>
       </c>
       <c r="C62" t="n">
-        <v>13500.0</v>
+        <v>7641.0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>7423.0</v>
+        <v>129239.0</v>
       </c>
       <c r="B63" t="n">
-        <v>7448.0</v>
+        <v>5015.0</v>
       </c>
       <c r="C63" t="n">
-        <v>10839.0</v>
+        <v>9401.0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>27060.0</v>
+        <v>94874.0</v>
       </c>
       <c r="B64" t="n">
-        <v>7598.0</v>
+        <v>5606.0</v>
       </c>
       <c r="C64" t="n">
-        <v>9525.0</v>
+        <v>10677.0</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>383849.0</v>
+        <v>162275.0</v>
       </c>
       <c r="B65" t="n">
-        <v>9113.0</v>
+        <v>3486.0</v>
       </c>
       <c r="C65" t="n">
-        <v>10254.0</v>
+        <v>7861.0</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>87250.0</v>
+        <v>28505.0</v>
       </c>
       <c r="B66" t="n">
-        <v>10600.0</v>
+        <v>5157.0</v>
       </c>
       <c r="C66" t="n">
-        <v>11338.0</v>
+        <v>7892.0</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>296659.0</v>
+        <v>149651.0</v>
       </c>
       <c r="B67" t="n">
-        <v>10469.0</v>
+        <v>4246.0</v>
       </c>
       <c r="C67" t="n">
-        <v>13537.0</v>
+        <v>7701.0</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>194982.0</v>
+        <v>13430.0</v>
       </c>
       <c r="B68" t="n">
-        <v>7572.0</v>
+        <v>5706.0</v>
       </c>
       <c r="C68" t="n">
-        <v>12367.0</v>
+        <v>7479.0</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>391230.0</v>
+        <v>7280.0</v>
       </c>
       <c r="B69" t="n">
-        <v>9073.0</v>
+        <v>4981.0</v>
       </c>
       <c r="C69" t="n">
-        <v>12181.0</v>
+        <v>7117.0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>185223.0</v>
+        <v>180055.0</v>
       </c>
       <c r="B70" t="n">
-        <v>12047.0</v>
+        <v>979.0</v>
       </c>
       <c r="C70" t="n">
-        <v>14698.0</v>
+        <v>7740.0</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>286380.0</v>
+        <v>188406.0</v>
       </c>
       <c r="B71" t="n">
-        <v>11084.0</v>
+        <v>2231.0</v>
       </c>
       <c r="C71" t="n">
-        <v>14087.0</v>
+        <v>10415.0</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>275237.0</v>
+        <v>186513.0</v>
       </c>
       <c r="B72" t="n">
-        <v>13752.0</v>
+        <v>3542.0</v>
       </c>
       <c r="C72" t="n">
-        <v>13462.0</v>
+        <v>8027.0</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>308589.0</v>
+        <v>29356.0</v>
       </c>
       <c r="B73" t="n">
-        <v>10892.0</v>
+        <v>5127.0</v>
       </c>
       <c r="C73" t="n">
-        <v>12326.0</v>
+        <v>10498.0</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>180899.0</v>
+        <v>80032.0</v>
       </c>
       <c r="B74" t="n">
-        <v>9026.0</v>
+        <v>5436.0</v>
       </c>
       <c r="C74" t="n">
-        <v>13768.0</v>
+        <v>7722.0</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>301444.0</v>
+        <v>101055.0</v>
       </c>
       <c r="B75" t="n">
-        <v>7409.0</v>
+        <v>5670.0</v>
       </c>
       <c r="C75" t="n">
-        <v>12643.0</v>
+        <v>8486.0</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>296345.0</v>
+        <v>187518.0</v>
       </c>
       <c r="B76" t="n">
-        <v>7097.0</v>
+        <v>663.0</v>
       </c>
       <c r="C76" t="n">
-        <v>12495.0</v>
+        <v>6135.0</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>278684.0</v>
+        <v>7502.0</v>
       </c>
       <c r="B77" t="n">
-        <v>7146.0</v>
+        <v>4387.0</v>
       </c>
       <c r="C77" t="n">
-        <v>13637.0</v>
+        <v>7304.0</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>134333.0</v>
+        <v>171799.0</v>
       </c>
       <c r="B78" t="n">
-        <v>10172.0</v>
+        <v>5199.0</v>
       </c>
       <c r="C78" t="n">
-        <v>15494.0</v>
+        <v>7621.0</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>322914.0</v>
+        <v>184277.0</v>
       </c>
       <c r="B79" t="n">
-        <v>11409.0</v>
+        <v>3203.0</v>
       </c>
       <c r="C79" t="n">
-        <v>14570.0</v>
+        <v>8744.0</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>90911.0</v>
+        <v>7135.0</v>
       </c>
       <c r="B80" t="n">
-        <v>11070.0</v>
+        <v>5636.0</v>
       </c>
       <c r="C80" t="n">
-        <v>13114.0</v>
+        <v>6804.0</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>321670.0</v>
+        <v>57426.0</v>
       </c>
       <c r="B81" t="n">
-        <v>11429.0</v>
+        <v>5128.0</v>
       </c>
       <c r="C81" t="n">
-        <v>13334.0</v>
+        <v>9005.0</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>394816.0</v>
+        <v>176634.0</v>
       </c>
       <c r="B82" t="n">
-        <v>6056.0</v>
+        <v>1885.0</v>
       </c>
       <c r="C82" t="n">
-        <v>10538.0</v>
+        <v>7320.0</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>288179.0</v>
+        <v>19681.0</v>
       </c>
       <c r="B83" t="n">
-        <v>12387.0</v>
+        <v>5660.0</v>
       </c>
       <c r="C83" t="n">
-        <v>9044.0</v>
+        <v>6827.0</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>206143.0</v>
+        <v>7616.0</v>
       </c>
       <c r="B84" t="n">
-        <v>8198.0</v>
+        <v>5931.0</v>
       </c>
       <c r="C84" t="n">
-        <v>11352.0</v>
+        <v>6761.0</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>141159.0</v>
+        <v>192737.0</v>
       </c>
       <c r="B85" t="n">
-        <v>12739.0</v>
+        <v>1401.0</v>
       </c>
       <c r="C85" t="n">
-        <v>13807.0</v>
+        <v>8362.0</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>93306.0</v>
+        <v>166321.0</v>
       </c>
       <c r="B86" t="n">
-        <v>6744.0</v>
+        <v>3094.0</v>
       </c>
       <c r="C86" t="n">
-        <v>13050.0</v>
+        <v>7700.0</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>84055.0</v>
+        <v>108373.0</v>
       </c>
       <c r="B87" t="n">
-        <v>9225.0</v>
+        <v>4655.0</v>
       </c>
       <c r="C87" t="n">
-        <v>14373.0</v>
+        <v>7828.0</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>16583.0</v>
+        <v>160086.0</v>
       </c>
       <c r="B88" t="n">
-        <v>8834.0</v>
+        <v>4327.0</v>
       </c>
       <c r="C88" t="n">
-        <v>11819.0</v>
+        <v>8221.0</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>15632.0</v>
+        <v>34978.0</v>
       </c>
       <c r="B89" t="n">
-        <v>10473.0</v>
+        <v>5086.0</v>
       </c>
       <c r="C89" t="n">
-        <v>12115.0</v>
+        <v>7461.0</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>108769.0</v>
+        <v>121946.0</v>
       </c>
       <c r="B90" t="n">
-        <v>11870.0</v>
+        <v>3681.0</v>
       </c>
       <c r="C90" t="n">
-        <v>14340.0</v>
+        <v>8827.0</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>75017.0</v>
+        <v>155497.0</v>
       </c>
       <c r="B91" t="n">
-        <v>11209.0</v>
+        <v>4297.0</v>
       </c>
       <c r="C91" t="n">
-        <v>15996.0</v>
+        <v>8173.0</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>52024.0</v>
+        <v>44685.0</v>
       </c>
       <c r="B92" t="n">
-        <v>13264.0</v>
+        <v>5847.0</v>
       </c>
       <c r="C92" t="n">
-        <v>12415.0</v>
+        <v>7986.0</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>22426.0</v>
+        <v>97633.0</v>
       </c>
       <c r="B93" t="n">
-        <v>10007.0</v>
+        <v>5379.0</v>
       </c>
       <c r="C93" t="n">
-        <v>11905.0</v>
+        <v>8259.0</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>182652.0</v>
+        <v>42531.0</v>
       </c>
       <c r="B94" t="n">
-        <v>10070.0</v>
+        <v>6178.0</v>
       </c>
       <c r="C94" t="n">
-        <v>10765.0</v>
+        <v>8549.0</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>14877.0</v>
+        <v>10655.0</v>
       </c>
       <c r="B95" t="n">
-        <v>10980.0</v>
+        <v>6201.0</v>
       </c>
       <c r="C95" t="n">
-        <v>11832.0</v>
+        <v>7398.0</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>184243.0</v>
+        <v>170209.0</v>
       </c>
       <c r="B96" t="n">
-        <v>4114.0</v>
+        <v>3768.0</v>
       </c>
       <c r="C96" t="n">
-        <v>12780.0</v>
+        <v>8829.0</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>167844.0</v>
+        <v>182474.0</v>
       </c>
       <c r="B97" t="n">
-        <v>3981.0</v>
+        <v>3018.0</v>
       </c>
       <c r="C97" t="n">
-        <v>11758.0</v>
+        <v>7962.0</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>197714.0</v>
+        <v>72093.0</v>
       </c>
       <c r="B98" t="n">
-        <v>1465.0</v>
+        <v>4556.0</v>
       </c>
       <c r="C98" t="n">
-        <v>11342.0</v>
+        <v>15780.0</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>108869.0</v>
+        <v>62959.0</v>
       </c>
       <c r="B99" t="n">
-        <v>5453.0</v>
+        <v>4754.0</v>
       </c>
       <c r="C99" t="n">
-        <v>11802.0</v>
+        <v>11393.0</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>7276.0</v>
+        <v>6892.0</v>
       </c>
       <c r="B100" t="n">
-        <v>5832.0</v>
+        <v>4736.0</v>
       </c>
       <c r="C100" t="n">
-        <v>10744.0</v>
+        <v>7053.0</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>175115.0</v>
+        <v>34654.0</v>
       </c>
       <c r="B101" t="n">
-        <v>2000.0</v>
+        <v>5734.0</v>
       </c>
       <c r="C101" t="n">
-        <v>9158.0</v>
+        <v>7513.0</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>125674.0</v>
+        <v>178638.0</v>
       </c>
       <c r="B102" t="n">
-        <v>4255.0</v>
+        <v>1217.0</v>
       </c>
       <c r="C102" t="n">
-        <v>10981.0</v>
+        <v>5869.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inserita la relazione in Latex
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -474,7 +474,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J152"/>
+  <dimension ref="A1:J201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
@@ -513,1663 +513,2202 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1350600.0</v>
+        <v>4.19116E7</v>
       </c>
       <c r="B2" t="n">
-        <v>700700.0</v>
+        <v>2205000.0</v>
       </c>
       <c r="C2" t="n">
-        <v>1054300.0</v>
+        <v>2878000.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>6371700.0</v>
+        <v>4.424549E8</v>
       </c>
       <c r="B3" t="n">
-        <v>183200.0</v>
+        <v>956600.0</v>
       </c>
       <c r="C3" t="n">
-        <v>118400.0</v>
+        <v>1308300.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3587100.0</v>
+        <v>4.57155E7</v>
       </c>
       <c r="B4" t="n">
-        <v>88700.0</v>
+        <v>393000.0</v>
       </c>
       <c r="C4" t="n">
-        <v>114700.0</v>
+        <v>1589500.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4718000.0</v>
+        <v>4.33557E7</v>
       </c>
       <c r="B5" t="n">
-        <v>103200.0</v>
+        <v>448200.0</v>
       </c>
       <c r="C5" t="n">
-        <v>177400.0</v>
+        <v>1338300.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>8644900.0</v>
+        <v>5.023907E8</v>
       </c>
       <c r="B6" t="n">
-        <v>66600.0</v>
+        <v>352500.0</v>
       </c>
       <c r="C6" t="n">
-        <v>107600.0</v>
+        <v>635700.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>3811100.0</v>
+        <v>1.116291E8</v>
       </c>
       <c r="B7" t="n">
-        <v>146600.0</v>
+        <v>512900.0</v>
       </c>
       <c r="C7" t="n">
-        <v>146300.0</v>
+        <v>568900.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2812800.0</v>
+        <v>5.183075E8</v>
       </c>
       <c r="B8" t="n">
-        <v>149100.0</v>
+        <v>184400.0</v>
       </c>
       <c r="C8" t="n">
-        <v>68500.0</v>
+        <v>300500.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>531900.0</v>
+        <v>1.518528E8</v>
       </c>
       <c r="B9" t="n">
-        <v>20800.0</v>
+        <v>119500.0</v>
       </c>
       <c r="C9" t="n">
-        <v>108600.0</v>
+        <v>501700.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1888300.0</v>
+        <v>4.876676E8</v>
       </c>
       <c r="B10" t="n">
-        <v>34700.0</v>
+        <v>101900.0</v>
       </c>
       <c r="C10" t="n">
-        <v>158700.0</v>
+        <v>417600.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2376100.0</v>
+        <v>1.184403E8</v>
       </c>
       <c r="B11" t="n">
-        <v>121000.0</v>
+        <v>107700.0</v>
       </c>
       <c r="C11" t="n">
-        <v>89600.0</v>
+        <v>382400.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1772800.0</v>
+        <v>3.809121E8</v>
       </c>
       <c r="B12" t="n">
-        <v>50600.0</v>
+        <v>124200.0</v>
       </c>
       <c r="C12" t="n">
-        <v>211900.0</v>
+        <v>304300.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>2487800.0</v>
+        <v>4.676851E8</v>
       </c>
       <c r="B13" t="n">
-        <v>51600.0</v>
+        <v>76200.0</v>
       </c>
       <c r="C13" t="n">
-        <v>74400.0</v>
+        <v>281700.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>4311500.0</v>
+        <v>4.629554E8</v>
       </c>
       <c r="B14" t="n">
-        <v>30050.0</v>
+        <v>179900.0</v>
       </c>
       <c r="C14" t="n">
-        <v>65500.0</v>
+        <v>473800.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>2936200.0</v>
+        <v>4.736431E8</v>
       </c>
       <c r="B15" t="n">
-        <v>32750.0</v>
+        <v>101900.0</v>
       </c>
       <c r="C15" t="n">
-        <v>171100.0</v>
+        <v>213600.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1218300.0</v>
+        <v>9.538E7</v>
       </c>
       <c r="B16" t="n">
-        <v>37250.0</v>
+        <v>110300.0</v>
       </c>
       <c r="C16" t="n">
-        <v>133900.0</v>
+        <v>374900.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1440100.0</v>
+        <v>1.43258E7</v>
       </c>
       <c r="B17" t="n">
-        <v>29500.0</v>
+        <v>177700.0</v>
       </c>
       <c r="C17" t="n">
-        <v>124500.0</v>
+        <v>390300.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>33200.0</v>
+        <v>4.08614E8</v>
       </c>
       <c r="B18" t="n">
-        <v>15950.0</v>
+        <v>145700.0</v>
       </c>
       <c r="C18" t="n">
-        <v>45700.0</v>
+        <v>400300.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>2725.0</v>
+        <v>5.254209E8</v>
       </c>
       <c r="B19" t="n">
-        <v>21200.0</v>
+        <v>123100.0</v>
       </c>
       <c r="C19" t="n">
-        <v>24300.0</v>
+        <v>293000.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>53300.0</v>
+        <v>1.33137E7</v>
       </c>
       <c r="B20" t="n">
-        <v>27200.0</v>
+        <v>122200.0</v>
       </c>
       <c r="C20" t="n">
-        <v>26200.0</v>
+        <v>465400.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>2288900.0</v>
+        <v>4.418679E8</v>
       </c>
       <c r="B21" t="n">
-        <v>15650.0</v>
+        <v>128800.0</v>
       </c>
       <c r="C21" t="n">
-        <v>17550.0</v>
+        <v>657900.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1453900.0</v>
+        <v>6.177091E8</v>
       </c>
       <c r="B22" t="n">
-        <v>35850.0</v>
+        <v>83300.0</v>
       </c>
       <c r="C22" t="n">
-        <v>25800.0</v>
+        <v>425900.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>2246200.0</v>
+        <v>8.536E7</v>
       </c>
       <c r="B23" t="n">
-        <v>34500.0</v>
+        <v>178300.0</v>
       </c>
       <c r="C23" t="n">
-        <v>35200.0</v>
+        <v>447100.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1293600.0</v>
+        <v>4.452751E8</v>
       </c>
       <c r="B24" t="n">
-        <v>95750.0</v>
+        <v>103300.0</v>
       </c>
       <c r="C24" t="n">
-        <v>24800.0</v>
+        <v>328600.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>530400.0</v>
+        <v>5.085187E8</v>
       </c>
       <c r="B25" t="n">
-        <v>48050.0</v>
+        <v>111400.0</v>
       </c>
       <c r="C25" t="n">
-        <v>45300.0</v>
+        <v>218100.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1650600.0</v>
+        <v>2258700.0</v>
       </c>
       <c r="B26" t="n">
-        <v>11766.0</v>
+        <v>119400.0</v>
       </c>
       <c r="C26" t="n">
-        <v>24000.0</v>
+        <v>601100.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>349300.0</v>
+        <v>1.483407E8</v>
       </c>
       <c r="B27" t="n">
-        <v>11150.0</v>
+        <v>152200.0</v>
       </c>
       <c r="C27" t="n">
-        <v>27400.0</v>
+        <v>1005800.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1486900.0</v>
+        <v>5.447902E8</v>
       </c>
       <c r="B28" t="n">
-        <v>7666.0</v>
+        <v>91600.0</v>
       </c>
       <c r="C28" t="n">
-        <v>24700.0</v>
+        <v>523400.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1599700.0</v>
+        <v>2.778904E8</v>
       </c>
       <c r="B29" t="n">
-        <v>14800.0</v>
+        <v>109400.0</v>
       </c>
       <c r="C29" t="n">
-        <v>35400.0</v>
+        <v>480900.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>1174700.0</v>
+        <v>6.08581E7</v>
       </c>
       <c r="B30" t="n">
-        <v>9100.0</v>
+        <v>42500.0</v>
       </c>
       <c r="C30" t="n">
-        <v>32300.0</v>
+        <v>437000.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>1386100.0</v>
+        <v>3.473675E8</v>
       </c>
       <c r="B31" t="n">
-        <v>10350.0</v>
+        <v>110000.0</v>
       </c>
       <c r="C31" t="n">
-        <v>24800.0</v>
+        <v>406900.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>635800.0</v>
+        <v>3.975247E8</v>
       </c>
       <c r="B32" t="n">
-        <v>3220933.0</v>
+        <v>122200.0</v>
       </c>
       <c r="C32" t="n">
-        <v>25600.0</v>
+        <v>586200.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1585300.0</v>
+        <v>4.267524E8</v>
       </c>
       <c r="B33" t="n">
-        <v>7166.0</v>
+        <v>100000.0</v>
       </c>
       <c r="C33" t="n">
-        <v>24300.0</v>
+        <v>316100.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>757100.0</v>
+        <v>2.848462E8</v>
       </c>
       <c r="B34" t="n">
-        <v>11450.0</v>
+        <v>114500.0</v>
       </c>
       <c r="C34" t="n">
-        <v>25400.0</v>
+        <v>327700.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>1638100.0</v>
+        <v>2.69871E7</v>
       </c>
       <c r="B35" t="n">
-        <v>6900.0</v>
+        <v>110000.0</v>
       </c>
       <c r="C35" t="n">
-        <v>25900.0</v>
+        <v>410000.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>3023700.0</v>
+        <v>1.523389E8</v>
       </c>
       <c r="B36" t="n">
-        <v>21066.0</v>
+        <v>144700.0</v>
       </c>
       <c r="C36" t="n">
-        <v>52000.0</v>
+        <v>342400.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1196200.0</v>
+        <v>4.557931E8</v>
       </c>
       <c r="B37" t="n">
-        <v>12450.0</v>
+        <v>190400.0</v>
       </c>
       <c r="C37" t="n">
-        <v>156100.0</v>
+        <v>236300.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>1855700.0</v>
+        <v>1.764468E8</v>
       </c>
       <c r="B38" t="n">
-        <v>26400.0</v>
+        <v>189600.0</v>
       </c>
       <c r="C38" t="n">
-        <v>37300.0</v>
+        <v>465000.0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>251300.0</v>
+        <v>201200.0</v>
       </c>
       <c r="B39" t="n">
-        <v>13733.0</v>
+        <v>81200.0</v>
       </c>
       <c r="C39" t="n">
-        <v>30300.0</v>
+        <v>671700.0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>2296700.0</v>
+        <v>1.755002E8</v>
       </c>
       <c r="B40" t="n">
-        <v>10650.0</v>
+        <v>161200.0</v>
       </c>
       <c r="C40" t="n">
-        <v>27200.0</v>
+        <v>479500.0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>287500.0</v>
+        <v>9.56236E7</v>
       </c>
       <c r="B41" t="n">
-        <v>7100.0</v>
+        <v>201700.0</v>
       </c>
       <c r="C41" t="n">
-        <v>74100.0</v>
+        <v>338200.0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>2217400.0</v>
+        <v>4.692122E8</v>
       </c>
       <c r="B42" t="n">
-        <v>9300.0</v>
+        <v>130200.0</v>
       </c>
       <c r="C42" t="n">
-        <v>29700.0</v>
+        <v>206800.0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>1321400.0</v>
+        <v>4.764432E8</v>
       </c>
       <c r="B43" t="n">
-        <v>11650.0</v>
+        <v>80600.0</v>
       </c>
       <c r="C43" t="n">
-        <v>35500.0</v>
+        <v>434300.0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>858500.0</v>
+        <v>7.34861E7</v>
       </c>
       <c r="B44" t="n">
-        <v>17100.0</v>
+        <v>207500.0</v>
       </c>
       <c r="C44" t="n">
-        <v>36600.0</v>
+        <v>376700.0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>1867500.0</v>
+        <v>4.306535E8</v>
       </c>
       <c r="B45" t="n">
-        <v>10766.0</v>
+        <v>115300.0</v>
       </c>
       <c r="C45" t="n">
-        <v>31300.0</v>
+        <v>283700.0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>1777700.0</v>
+        <v>4.751782E8</v>
       </c>
       <c r="B46" t="n">
-        <v>13166.0</v>
+        <v>100300.0</v>
       </c>
       <c r="C46" t="n">
-        <v>36500.0</v>
+        <v>214500.0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>199800.0</v>
+        <v>4.343924E8</v>
       </c>
       <c r="B47" t="n">
-        <v>23700.0</v>
+        <v>80400.0</v>
       </c>
       <c r="C47" t="n">
-        <v>22900.0</v>
+        <v>349300.0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>254600.0</v>
+        <v>4.018256E8</v>
       </c>
       <c r="B48" t="n">
-        <v>7400.0</v>
+        <v>73300.0</v>
       </c>
       <c r="C48" t="n">
-        <v>29400.0</v>
+        <v>344900.0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>279700.0</v>
+        <v>3.157459E8</v>
       </c>
       <c r="B49" t="n">
-        <v>15200.0</v>
+        <v>137600.0</v>
       </c>
       <c r="C49" t="n">
-        <v>63500.0</v>
+        <v>537800.0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>156700.0</v>
+        <v>2.163802E8</v>
       </c>
       <c r="B50" t="n">
-        <v>14966.0</v>
+        <v>99900.0</v>
       </c>
       <c r="C50" t="n">
-        <v>33900.0</v>
+        <v>377200.0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>593600.0</v>
+        <v>4.244308E8</v>
       </c>
       <c r="B51" t="n">
-        <v>12100.0</v>
+        <v>71900.0</v>
       </c>
       <c r="C51" t="n">
-        <v>29400.0</v>
+        <v>484300.0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>1231400.0</v>
+        <v>2.90431E7</v>
       </c>
       <c r="B52" t="n">
-        <v>10433.0</v>
+        <v>70700.0</v>
       </c>
       <c r="C52" t="n">
-        <v>119400.0</v>
+        <v>383300.0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>2240700.0</v>
+        <v>1.271117E8</v>
       </c>
       <c r="B53" t="n">
-        <v>16700.0</v>
+        <v>90500.0</v>
       </c>
       <c r="C53" t="n">
-        <v>33900.0</v>
+        <v>380300.0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>1465400.0</v>
+        <v>4.763054E8</v>
       </c>
       <c r="B54" t="n">
-        <v>9966.0</v>
+        <v>104400.0</v>
       </c>
       <c r="C54" t="n">
-        <v>30400.0</v>
+        <v>216900.0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>1201100.0</v>
+        <v>4.354668E8</v>
       </c>
       <c r="B55" t="n">
-        <v>6733.0</v>
+        <v>145000.0</v>
       </c>
       <c r="C55" t="n">
-        <v>22100.0</v>
+        <v>286100.0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>18350.0</v>
+        <v>1.97274E7</v>
       </c>
       <c r="B56" t="n">
-        <v>8566.0</v>
+        <v>108600.0</v>
       </c>
       <c r="C56" t="n">
-        <v>18850.0</v>
+        <v>394200.0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>557000.0</v>
+        <v>4.891647E8</v>
       </c>
       <c r="B57" t="n">
-        <v>7600.0</v>
+        <v>112300.0</v>
       </c>
       <c r="C57" t="n">
-        <v>30600.0</v>
+        <v>215000.0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>1883200.0</v>
+        <v>1.008594E8</v>
       </c>
       <c r="B58" t="n">
-        <v>6866.0</v>
+        <v>195800.0</v>
       </c>
       <c r="C58" t="n">
-        <v>35800.0</v>
+        <v>315700.0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>462600.0</v>
+        <v>2.800487E8</v>
       </c>
       <c r="B59" t="n">
-        <v>9133.0</v>
+        <v>120800.0</v>
       </c>
       <c r="C59" t="n">
-        <v>20700.0</v>
+        <v>487100.0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>1131600.0</v>
+        <v>5.107708E8</v>
       </c>
       <c r="B60" t="n">
-        <v>10733.0</v>
+        <v>119100.0</v>
       </c>
       <c r="C60" t="n">
-        <v>22600.0</v>
+        <v>213600.0</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>184700.0</v>
+        <v>1.631646E8</v>
       </c>
       <c r="B61" t="n">
-        <v>10450.0</v>
+        <v>107500.0</v>
       </c>
       <c r="C61" t="n">
-        <v>35600.0</v>
+        <v>330900.0</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>203500.0</v>
+        <v>3.455055E8</v>
       </c>
       <c r="B62" t="n">
-        <v>12200.0</v>
+        <v>134400.0</v>
       </c>
       <c r="C62" t="n">
-        <v>29300.0</v>
+        <v>444800.0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>1374400.0</v>
+        <v>1.13962E7</v>
       </c>
       <c r="B63" t="n">
-        <v>7400.0</v>
+        <v>117000.0</v>
       </c>
       <c r="C63" t="n">
-        <v>22800.0</v>
+        <v>372000.0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>1561200.0</v>
+        <v>3.313005E8</v>
       </c>
       <c r="B64" t="n">
-        <v>8566.0</v>
+        <v>136300.0</v>
       </c>
       <c r="C64" t="n">
-        <v>15850.0</v>
+        <v>375900.0</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>2410800.0</v>
+        <v>4.79322E8</v>
       </c>
       <c r="B65" t="n">
-        <v>7000.0</v>
+        <v>131900.0</v>
       </c>
       <c r="C65" t="n">
-        <v>20900.0</v>
+        <v>205900.0</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>154700.0</v>
+        <v>1879500.0</v>
       </c>
       <c r="B66" t="n">
-        <v>18400.0</v>
+        <v>90500.0</v>
       </c>
       <c r="C66" t="n">
-        <v>25800.0</v>
+        <v>301400.0</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>1840500.0</v>
+        <v>5285200.0</v>
       </c>
       <c r="B67" t="n">
-        <v>10650.0</v>
+        <v>54000.0</v>
       </c>
       <c r="C67" t="n">
-        <v>26900.0</v>
+        <v>341800.0</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>980500.0</v>
+        <v>3.684604E8</v>
       </c>
       <c r="B68" t="n">
-        <v>23633.0</v>
+        <v>164100.0</v>
       </c>
       <c r="C68" t="n">
-        <v>22700.0</v>
+        <v>636900.0</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>987200.0</v>
+        <v>8.187236E8</v>
       </c>
       <c r="B69" t="n">
-        <v>10200.0</v>
+        <v>104300.0</v>
       </c>
       <c r="C69" t="n">
-        <v>17100.0</v>
+        <v>273200.0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>553500.0</v>
+        <v>169600.0</v>
       </c>
       <c r="B70" t="n">
-        <v>13733.0</v>
+        <v>136500.0</v>
       </c>
       <c r="C70" t="n">
-        <v>25500.0</v>
+        <v>450800.0</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>1697800.0</v>
+        <v>2.780318E8</v>
       </c>
       <c r="B71" t="n">
-        <v>15350.0</v>
+        <v>175400.0</v>
       </c>
       <c r="C71" t="n">
-        <v>26400.0</v>
+        <v>898300.0</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>41500.0</v>
+        <v>6.037346E8</v>
       </c>
       <c r="B72" t="n">
-        <v>9233.0</v>
+        <v>92000.0</v>
       </c>
       <c r="C72" t="n">
-        <v>27000.0</v>
+        <v>456400.0</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>370200.0</v>
+        <v>9.127573E8</v>
       </c>
       <c r="B73" t="n">
-        <v>11800.0</v>
+        <v>93500.0</v>
       </c>
       <c r="C73" t="n">
-        <v>15300.0</v>
+        <v>266300.0</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>1046200.0</v>
+        <v>5.149141E8</v>
       </c>
       <c r="B74" t="n">
-        <v>11400.0</v>
+        <v>78300.0</v>
       </c>
       <c r="C74" t="n">
-        <v>21800.0</v>
+        <v>526300.0</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>1517600.0</v>
+        <v>1.049331E8</v>
       </c>
       <c r="B75" t="n">
-        <v>5275.0</v>
+        <v>111100.0</v>
       </c>
       <c r="C75" t="n">
-        <v>13100.0</v>
+        <v>464300.0</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>98700.0</v>
+        <v>5801800.0</v>
       </c>
       <c r="B76" t="n">
-        <v>9833.0</v>
+        <v>64800.0</v>
       </c>
       <c r="C76" t="n">
-        <v>26300.0</v>
+        <v>349400.0</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>843100.0</v>
+        <v>7.366305E8</v>
       </c>
       <c r="B77" t="n">
-        <v>11866.0</v>
+        <v>88500.0</v>
       </c>
       <c r="C77" t="n">
-        <v>18300.0</v>
+        <v>244300.0</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>67300.0</v>
+        <v>6.756578E8</v>
       </c>
       <c r="B78" t="n">
-        <v>27650.0</v>
+        <v>170200.0</v>
       </c>
       <c r="C78" t="n">
-        <v>25600.0</v>
+        <v>347300.0</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>1643100.0</v>
+        <v>1.59045E7</v>
       </c>
       <c r="B79" t="n">
-        <v>6833.0</v>
+        <v>125200.0</v>
       </c>
       <c r="C79" t="n">
-        <v>26100.0</v>
+        <v>385400.0</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>3800.0</v>
+        <v>7.328641E8</v>
       </c>
       <c r="B80" t="n">
-        <v>7066.0</v>
+        <v>137200.0</v>
       </c>
       <c r="C80" t="n">
-        <v>25000.0</v>
+        <v>373000.0</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>2324700.0</v>
+        <v>6656200.0</v>
       </c>
       <c r="B81" t="n">
-        <v>15950.0</v>
+        <v>147900.0</v>
       </c>
       <c r="C81" t="n">
-        <v>24400.0</v>
+        <v>397500.0</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>1060600.0</v>
+        <v>8.232562E8</v>
       </c>
       <c r="B82" t="n">
-        <v>12800.0</v>
+        <v>79700.0</v>
       </c>
       <c r="C82" t="n">
-        <v>16600.0</v>
+        <v>252400.0</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>411500.0</v>
+        <v>6.08428E8</v>
       </c>
       <c r="B83" t="n">
-        <v>12600.0</v>
+        <v>211500.0</v>
       </c>
       <c r="C83" t="n">
-        <v>24300.0</v>
+        <v>530100.0</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>341600.0</v>
+        <v>4.443732E8</v>
       </c>
       <c r="B84" t="n">
-        <v>8600.0</v>
+        <v>245200.0</v>
       </c>
       <c r="C84" t="n">
-        <v>29700.0</v>
+        <v>505800.0</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>1479000.0</v>
+        <v>1.98676E7</v>
       </c>
       <c r="B85" t="n">
-        <v>17100.0</v>
+        <v>142500.0</v>
       </c>
       <c r="C85" t="n">
-        <v>23500.0</v>
+        <v>403200.0</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>2219200.0</v>
+        <v>5.310439E8</v>
       </c>
       <c r="B86" t="n">
-        <v>12600.0</v>
+        <v>142200.0</v>
       </c>
       <c r="C86" t="n">
-        <v>24100.0</v>
+        <v>320200.0</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>758100.0</v>
+        <v>1.798152E8</v>
       </c>
       <c r="B87" t="n">
-        <v>13550.0</v>
+        <v>68700.0</v>
       </c>
       <c r="C87" t="n">
-        <v>29800.0</v>
+        <v>550600.0</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>403200.0</v>
+        <v>1.255323E8</v>
       </c>
       <c r="B88" t="n">
-        <v>14100.0</v>
+        <v>137300.0</v>
       </c>
       <c r="C88" t="n">
-        <v>22700.0</v>
+        <v>396000.0</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>876700.0</v>
+        <v>1.479636E8</v>
       </c>
       <c r="B89" t="n">
-        <v>6800.0</v>
+        <v>137300.0</v>
       </c>
       <c r="C89" t="n">
-        <v>19550.0</v>
+        <v>427200.0</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>17450.0</v>
+        <v>3.291839E8</v>
       </c>
       <c r="B90" t="n">
-        <v>7466.0</v>
+        <v>93800.0</v>
       </c>
       <c r="C90" t="n">
-        <v>16900.0</v>
+        <v>440200.0</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>426100.0</v>
+        <v>5.381998E8</v>
       </c>
       <c r="B91" t="n">
-        <v>10950.0</v>
+        <v>83000.0</v>
       </c>
       <c r="C91" t="n">
-        <v>58300.0</v>
+        <v>334400.0</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>821800.0</v>
+        <v>4.20894E7</v>
       </c>
       <c r="B92" t="n">
-        <v>13350.0</v>
+        <v>70800.0</v>
       </c>
       <c r="C92" t="n">
-        <v>26000.0</v>
+        <v>488500.0</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>341500.0</v>
+        <v>4.075703E8</v>
       </c>
       <c r="B93" t="n">
-        <v>26500.0</v>
+        <v>113200.0</v>
       </c>
       <c r="C93" t="n">
-        <v>26700.0</v>
+        <v>307300.0</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>1325500.0</v>
+        <v>8.82927E7</v>
       </c>
       <c r="B94" t="n">
-        <v>11050.0</v>
+        <v>175500.0</v>
       </c>
       <c r="C94" t="n">
-        <v>23000.0</v>
+        <v>395400.0</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>1777100.0</v>
+        <v>1.726156E8</v>
       </c>
       <c r="B95" t="n">
-        <v>12633.0</v>
+        <v>95400.0</v>
       </c>
       <c r="C95" t="n">
-        <v>24700.0</v>
+        <v>341600.0</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>223500.0</v>
+        <v>5.985403E8</v>
       </c>
       <c r="B96" t="n">
-        <v>10250.0</v>
+        <v>69400.0</v>
       </c>
       <c r="C96" t="n">
-        <v>28400.0</v>
+        <v>225200.0</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>1085600.0</v>
+        <v>2.575261E8</v>
       </c>
       <c r="B97" t="n">
-        <v>12800.0</v>
+        <v>77700.0</v>
       </c>
       <c r="C97" t="n">
-        <v>24100.0</v>
+        <v>503000.0</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>1385400.0</v>
+        <v>2.150641E8</v>
       </c>
       <c r="B98" t="n">
-        <v>23300.0</v>
+        <v>184400.0</v>
       </c>
       <c r="C98" t="n">
-        <v>23700.0</v>
+        <v>362700.0</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>16600.0</v>
+        <v>2.331142E8</v>
       </c>
       <c r="B99" t="n">
-        <v>14366.0</v>
+        <v>184700.0</v>
       </c>
       <c r="C99" t="n">
-        <v>31100.0</v>
+        <v>502800.0</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>368300.0</v>
+        <v>5.900741E8</v>
       </c>
       <c r="B100" t="n">
-        <v>9533.0</v>
+        <v>49800.0</v>
       </c>
       <c r="C100" t="n">
-        <v>29700.0</v>
+        <v>203300.0</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>2104500.0</v>
+        <v>3.80658E8</v>
       </c>
       <c r="B101" t="n">
-        <v>14666.0</v>
+        <v>78700.0</v>
       </c>
       <c r="C101" t="n">
-        <v>27600.0</v>
+        <v>408700.0</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>617100.0</v>
+        <v>2.960605E8</v>
       </c>
       <c r="B102" t="n">
-        <v>10200.0</v>
+        <v>114300.0</v>
       </c>
       <c r="C102" t="n">
-        <v>25800.0</v>
+        <v>371800.0</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>1731500.0</v>
+        <v>3.543615E8</v>
       </c>
       <c r="B103" t="n">
-        <v>11250.0</v>
+        <v>137900.0</v>
       </c>
       <c r="C103" t="n">
-        <v>25400.0</v>
+        <v>332900.0</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>2293300.0</v>
+        <v>4.04283E8</v>
       </c>
       <c r="B104" t="n">
-        <v>10400.0</v>
+        <v>124600.0</v>
       </c>
       <c r="C104" t="n">
-        <v>23400.0</v>
+        <v>432800.0</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>769900.0</v>
+        <v>4.250747E8</v>
       </c>
       <c r="B105" t="n">
-        <v>11450.0</v>
+        <v>273800.0</v>
       </c>
       <c r="C105" t="n">
-        <v>29100.0</v>
+        <v>424100.0</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>265100.0</v>
+        <v>1.126936E8</v>
       </c>
       <c r="B106" t="n">
-        <v>11000.0</v>
+        <v>113800.0</v>
       </c>
       <c r="C106" t="n">
-        <v>24000.0</v>
+        <v>357300.0</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>1571100.0</v>
+        <v>4.705279E8</v>
       </c>
       <c r="B107" t="n">
-        <v>10950.0</v>
+        <v>99400.0</v>
       </c>
       <c r="C107" t="n">
-        <v>30200.0</v>
+        <v>216800.0</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>261900.0</v>
+        <v>1.112476E8</v>
       </c>
       <c r="B108" t="n">
-        <v>10900.0</v>
+        <v>90200.0</v>
       </c>
       <c r="C108" t="n">
-        <v>22400.0</v>
+        <v>314300.0</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>533600.0</v>
+        <v>2.923353E8</v>
       </c>
       <c r="B109" t="n">
-        <v>13800.0</v>
+        <v>103600.0</v>
       </c>
       <c r="C109" t="n">
-        <v>25500.0</v>
+        <v>476100.0</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>510.0</v>
+        <v>4.59623E8</v>
       </c>
       <c r="B110" t="n">
-        <v>15450.0</v>
+        <v>108700.0</v>
       </c>
       <c r="C110" t="n">
-        <v>25700.0</v>
+        <v>201000.0</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>1295000.0</v>
+        <v>5.14428E7</v>
       </c>
       <c r="B111" t="n">
-        <v>17150.0</v>
+        <v>62700.0</v>
       </c>
       <c r="C111" t="n">
-        <v>26600.0</v>
+        <v>492700.0</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>20700.0</v>
+        <v>1.490407E8</v>
       </c>
       <c r="B112" t="n">
-        <v>14550.0</v>
+        <v>121200.0</v>
       </c>
       <c r="C112" t="n">
-        <v>28700.0</v>
+        <v>358200.0</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>2122700.0</v>
+        <v>6.78847E7</v>
       </c>
       <c r="B113" t="n">
-        <v>19300.0</v>
+        <v>91900.0</v>
       </c>
       <c r="C113" t="n">
-        <v>86000.0</v>
+        <v>346200.0</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>2038700.0</v>
+        <v>4.723846E8</v>
       </c>
       <c r="B114" t="n">
-        <v>18300.0</v>
+        <v>175900.0</v>
       </c>
       <c r="C114" t="n">
-        <v>23800.0</v>
+        <v>220300.0</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>1663100.0</v>
+        <v>4.685087E8</v>
       </c>
       <c r="B115" t="n">
-        <v>19700.0</v>
+        <v>97800.0</v>
       </c>
       <c r="C115" t="n">
-        <v>26200.0</v>
+        <v>216000.0</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>11650.0</v>
+        <v>2.646003E8</v>
       </c>
       <c r="B116" t="n">
-        <v>233166.0</v>
+        <v>86000.0</v>
       </c>
       <c r="C116" t="n">
-        <v>25700.0</v>
+        <v>554400.0</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>768100.0</v>
+        <v>4.492847E8</v>
       </c>
       <c r="B117" t="n">
-        <v>25250.0</v>
+        <v>97100.0</v>
       </c>
       <c r="C117" t="n">
-        <v>28800.0</v>
+        <v>370600.0</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>1678100.0</v>
+        <v>3.026384E8</v>
       </c>
       <c r="B118" t="n">
-        <v>9500.0</v>
+        <v>154900.0</v>
       </c>
       <c r="C118" t="n">
-        <v>28100.0</v>
+        <v>407600.0</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>2063500.0</v>
+        <v>4.837726E8</v>
       </c>
       <c r="B119" t="n">
-        <v>27600.0</v>
+        <v>105400.0</v>
       </c>
       <c r="C119" t="n">
-        <v>24200.0</v>
+        <v>227900.0</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>1578000.0</v>
+        <v>4.208179E8</v>
       </c>
       <c r="B120" t="n">
-        <v>12050.0</v>
+        <v>92900.0</v>
       </c>
       <c r="C120" t="n">
-        <v>24100.0</v>
+        <v>457600.0</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>2017700.0</v>
+        <v>2.325412E8</v>
       </c>
       <c r="B121" t="n">
-        <v>13800.0</v>
+        <v>92500.0</v>
       </c>
       <c r="C121" t="n">
-        <v>23700.0</v>
+        <v>424800.0</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>1750700.0</v>
+        <v>4.832641E8</v>
       </c>
       <c r="B122" t="n">
-        <v>10350.0</v>
+        <v>28600.0</v>
       </c>
       <c r="C122" t="n">
-        <v>24700.0</v>
+        <v>307400.0</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>1653000.0</v>
+        <v>2.393694E8</v>
       </c>
       <c r="B123" t="n">
-        <v>13600.0</v>
+        <v>169400.0</v>
       </c>
       <c r="C123" t="n">
-        <v>27500.0</v>
+        <v>368100.0</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>1610800.0</v>
+        <v>7.64975E7</v>
       </c>
       <c r="B124" t="n">
-        <v>12400.0</v>
+        <v>87500.0</v>
       </c>
       <c r="C124" t="n">
-        <v>20500.0</v>
+        <v>511700.0</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>105400.0</v>
+        <v>3.732792E8</v>
       </c>
       <c r="B125" t="n">
-        <v>9000.0</v>
+        <v>70500.0</v>
       </c>
       <c r="C125" t="n">
-        <v>30000.0</v>
+        <v>390700.0</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>2255100.0</v>
+        <v>1.88108E7</v>
       </c>
       <c r="B126" t="n">
-        <v>13800.0</v>
+        <v>105800.0</v>
       </c>
       <c r="C126" t="n">
-        <v>22300.0</v>
+        <v>343300.0</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>1897700.0</v>
+        <v>3.98413E8</v>
       </c>
       <c r="B127" t="n">
-        <v>12450.0</v>
+        <v>85900.0</v>
       </c>
       <c r="C127" t="n">
-        <v>24400.0</v>
+        <v>402000.0</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>1516100.0</v>
+        <v>4.1824E7</v>
       </c>
       <c r="B128" t="n">
-        <v>14333.0</v>
+        <v>113000.0</v>
       </c>
       <c r="C128" t="n">
-        <v>26600.0</v>
+        <v>404100.0</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>2234200.0</v>
+        <v>7.70056E7</v>
       </c>
       <c r="B129" t="n">
-        <v>10850.0</v>
+        <v>137400.0</v>
       </c>
       <c r="C129" t="n">
-        <v>24000.0</v>
+        <v>536100.0</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>1410600.0</v>
+        <v>4.691128E8</v>
       </c>
       <c r="B130" t="n">
-        <v>9175.0</v>
+        <v>115800.0</v>
       </c>
       <c r="C130" t="n">
-        <v>29400.0</v>
+        <v>234400.0</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>1566700.0</v>
+        <v>4.045178E8</v>
       </c>
       <c r="B131" t="n">
-        <v>10000.0</v>
+        <v>144200.0</v>
       </c>
       <c r="C131" t="n">
-        <v>26600.0</v>
+        <v>307200.0</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>1532800.0</v>
+        <v>3.299058E8</v>
       </c>
       <c r="B132" t="n">
-        <v>9333.0</v>
+        <v>110800.0</v>
       </c>
       <c r="C132" t="n">
-        <v>17900.0</v>
+        <v>359700.0</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>463400.0</v>
+        <v>4.363662E8</v>
       </c>
       <c r="B133" t="n">
-        <v>14950.0</v>
+        <v>172900.0</v>
       </c>
       <c r="C133" t="n">
-        <v>20800.0</v>
+        <v>361100.0</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>1468900.0</v>
+        <v>2.613955E8</v>
       </c>
       <c r="B134" t="n">
-        <v>7766.0</v>
+        <v>142000.0</v>
       </c>
       <c r="C134" t="n">
-        <v>15900.0</v>
+        <v>320700.0</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>2332500.0</v>
+        <v>3.468714E8</v>
       </c>
       <c r="B135" t="n">
-        <v>14800.0</v>
+        <v>140900.0</v>
       </c>
       <c r="C135" t="n">
-        <v>26300.0</v>
+        <v>357400.0</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>1923000.0</v>
+        <v>6014100.0</v>
       </c>
       <c r="B136" t="n">
-        <v>10750.0</v>
+        <v>73200.0</v>
       </c>
       <c r="C136" t="n">
-        <v>25900.0</v>
+        <v>353100.0</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>1316200.0</v>
+        <v>5.69382E7</v>
       </c>
       <c r="B137" t="n">
-        <v>14450.0</v>
+        <v>84100.0</v>
       </c>
       <c r="C137" t="n">
-        <v>43100.0</v>
+        <v>353500.0</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>1319600.0</v>
+        <v>2.283146E8</v>
       </c>
       <c r="B138" t="n">
-        <v>22450.0</v>
+        <v>99300.0</v>
       </c>
       <c r="C138" t="n">
-        <v>27100.0</v>
+        <v>367500.0</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>1988800.0</v>
+        <v>425300.0</v>
       </c>
       <c r="B139" t="n">
-        <v>6375.0</v>
+        <v>68000.0</v>
       </c>
       <c r="C139" t="n">
-        <v>21900.0</v>
+        <v>303200.0</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>1879500.0</v>
+        <v>1.277205E8</v>
       </c>
       <c r="B140" t="n">
-        <v>10350.0</v>
+        <v>125800.0</v>
       </c>
       <c r="C140" t="n">
-        <v>25900.0</v>
+        <v>293600.0</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>1692500.0</v>
+        <v>2.320594E8</v>
       </c>
       <c r="B141" t="n">
-        <v>10400.0</v>
+        <v>79600.0</v>
       </c>
       <c r="C141" t="n">
-        <v>21100.0</v>
+        <v>371800.0</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>1560500.0</v>
+        <v>2.44124E7</v>
       </c>
       <c r="B142" t="n">
-        <v>11033.0</v>
+        <v>171100.0</v>
       </c>
       <c r="C142" t="n">
-        <v>25700.0</v>
+        <v>324000.0</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>752700.0</v>
+        <v>4.418859E8</v>
       </c>
       <c r="B143" t="n">
-        <v>9400.0</v>
+        <v>175000.0</v>
       </c>
       <c r="C143" t="n">
-        <v>29200.0</v>
+        <v>299900.0</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>2652900.0</v>
+        <v>3.448668E8</v>
       </c>
       <c r="B144" t="n">
-        <v>4160.0</v>
+        <v>105500.0</v>
       </c>
       <c r="C144" t="n">
-        <v>18200.0</v>
+        <v>320600.0</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>83100.0</v>
+        <v>2.76612E8</v>
       </c>
       <c r="B145" t="n">
-        <v>10450.0</v>
+        <v>207000.0</v>
       </c>
       <c r="C145" t="n">
-        <v>30100.0</v>
+        <v>402100.0</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>214000.0</v>
+        <v>1.01149E7</v>
       </c>
       <c r="B146" t="n">
-        <v>11650.0</v>
+        <v>50300.0</v>
       </c>
       <c r="C146" t="n">
-        <v>25400.0</v>
+        <v>329600.0</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>6928500.0</v>
+        <v>4.520161E8</v>
       </c>
       <c r="B147" t="n">
-        <v>7800.0</v>
+        <v>118800.0</v>
       </c>
       <c r="C147" t="n">
-        <v>71400.0</v>
+        <v>439500.0</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>2790600.0</v>
+        <v>3.316355E8</v>
       </c>
       <c r="B148" t="n">
-        <v>11366.0</v>
+        <v>169100.0</v>
       </c>
       <c r="C148" t="n">
-        <v>24100.0</v>
+        <v>381600.0</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>3755900.0</v>
+        <v>2.92195E8</v>
       </c>
       <c r="B149" t="n">
-        <v>13400.0</v>
+        <v>79700.0</v>
       </c>
       <c r="C149" t="n">
-        <v>29400.0</v>
+        <v>516500.0</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>1696100.0</v>
+        <v>3.996818E8</v>
       </c>
       <c r="B150" t="n">
-        <v>11300.0</v>
+        <v>118900.0</v>
       </c>
       <c r="C150" t="n">
-        <v>22300.0</v>
+        <v>416800.0</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>24800.0</v>
+        <v>4.427807E8</v>
       </c>
       <c r="B151" t="n">
-        <v>16850.0</v>
+        <v>144700.0</v>
       </c>
       <c r="C151" t="n">
-        <v>31400.0</v>
+        <v>331400.0</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>669400.0</v>
+        <v>3.408252E8</v>
       </c>
       <c r="B152" t="n">
-        <v>12150.0</v>
+        <v>126600.0</v>
       </c>
       <c r="C152" t="n">
-        <v>31300.0</v>
+        <v>305000.0</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>9.19217E7</v>
+      </c>
+      <c r="B153" t="n">
+        <v>114500.0</v>
+      </c>
+      <c r="C153" t="n">
+        <v>522300.0</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>1.461673E8</v>
+      </c>
+      <c r="B154" t="n">
+        <v>127800.0</v>
+      </c>
+      <c r="C154" t="n">
+        <v>375200.0</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>7.78282E7</v>
+      </c>
+      <c r="B155" t="n">
+        <v>114600.0</v>
+      </c>
+      <c r="C155" t="n">
+        <v>430200.0</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>7.84026E7</v>
+      </c>
+      <c r="B156" t="n">
+        <v>94100.0</v>
+      </c>
+      <c r="C156" t="n">
+        <v>335800.0</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>3.15096E7</v>
+      </c>
+      <c r="B157" t="n">
+        <v>80800.0</v>
+      </c>
+      <c r="C157" t="n">
+        <v>320100.0</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>2.89124E7</v>
+      </c>
+      <c r="B158" t="n">
+        <v>63900.0</v>
+      </c>
+      <c r="C158" t="n">
+        <v>341900.0</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>4.250626E8</v>
+      </c>
+      <c r="B159" t="n">
+        <v>138600.0</v>
+      </c>
+      <c r="C159" t="n">
+        <v>320100.0</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>2.527745E8</v>
+      </c>
+      <c r="B160" t="n">
+        <v>91900.0</v>
+      </c>
+      <c r="C160" t="n">
+        <v>452900.0</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>4.740457E8</v>
+      </c>
+      <c r="B161" t="n">
+        <v>108900.0</v>
+      </c>
+      <c r="C161" t="n">
+        <v>210600.0</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>9786500.0</v>
+      </c>
+      <c r="B162" t="n">
+        <v>95300.0</v>
+      </c>
+      <c r="C162" t="n">
+        <v>285500.0</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>3.815675E8</v>
+      </c>
+      <c r="B163" t="n">
+        <v>200700.0</v>
+      </c>
+      <c r="C163" t="n">
+        <v>328300.0</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>9.94274E7</v>
+      </c>
+      <c r="B164" t="n">
+        <v>153800.0</v>
+      </c>
+      <c r="C164" t="n">
+        <v>375700.0</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>4.524E7</v>
+      </c>
+      <c r="B165" t="n">
+        <v>120600.0</v>
+      </c>
+      <c r="C165" t="n">
+        <v>464300.0</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>1.47354E8</v>
+      </c>
+      <c r="B166" t="n">
+        <v>116700.0</v>
+      </c>
+      <c r="C166" t="n">
+        <v>421900.0</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>8.7556E7</v>
+      </c>
+      <c r="B167" t="n">
+        <v>64300.0</v>
+      </c>
+      <c r="C167" t="n">
+        <v>378000.0</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>4.703977E8</v>
+      </c>
+      <c r="B168" t="n">
+        <v>115100.0</v>
+      </c>
+      <c r="C168" t="n">
+        <v>238800.0</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>4.258294E8</v>
+      </c>
+      <c r="B169" t="n">
+        <v>116400.0</v>
+      </c>
+      <c r="C169" t="n">
+        <v>542200.0</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>4.398222E8</v>
+      </c>
+      <c r="B170" t="n">
+        <v>130900.0</v>
+      </c>
+      <c r="C170" t="n">
+        <v>316500.0</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>1.97901E7</v>
+      </c>
+      <c r="B171" t="n">
+        <v>58200.0</v>
+      </c>
+      <c r="C171" t="n">
+        <v>338200.0</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>5.39286E7</v>
+      </c>
+      <c r="B172" t="n">
+        <v>99100.0</v>
+      </c>
+      <c r="C172" t="n">
+        <v>321000.0</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>3.169569E8</v>
+      </c>
+      <c r="B173" t="n">
+        <v>78700.0</v>
+      </c>
+      <c r="C173" t="n">
+        <v>546600.0</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>3.683131E8</v>
+      </c>
+      <c r="B174" t="n">
+        <v>126800.0</v>
+      </c>
+      <c r="C174" t="n">
+        <v>354100.0</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>1.876889E8</v>
+      </c>
+      <c r="B175" t="n">
+        <v>107500.0</v>
+      </c>
+      <c r="C175" t="n">
+        <v>461400.0</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>2.959635E8</v>
+      </c>
+      <c r="B176" t="n">
+        <v>121200.0</v>
+      </c>
+      <c r="C176" t="n">
+        <v>467800.0</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>2808000.0</v>
+      </c>
+      <c r="B177" t="n">
+        <v>85500.0</v>
+      </c>
+      <c r="C177" t="n">
+        <v>562900.0</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>4.694412E8</v>
+      </c>
+      <c r="B178" t="n">
+        <v>123100.0</v>
+      </c>
+      <c r="C178" t="n">
+        <v>208700.0</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>4.493829E8</v>
+      </c>
+      <c r="B179" t="n">
+        <v>99700.0</v>
+      </c>
+      <c r="C179" t="n">
+        <v>315300.0</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>4.273799E8</v>
+      </c>
+      <c r="B180" t="n">
+        <v>136200.0</v>
+      </c>
+      <c r="C180" t="n">
+        <v>321800.0</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>1.692402E8</v>
+      </c>
+      <c r="B181" t="n">
+        <v>204000.0</v>
+      </c>
+      <c r="C181" t="n">
+        <v>337600.0</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="n">
+        <v>6.41376E7</v>
+      </c>
+      <c r="B182" t="n">
+        <v>53600.0</v>
+      </c>
+      <c r="C182" t="n">
+        <v>368100.0</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="n">
+        <v>1.37347E7</v>
+      </c>
+      <c r="B183" t="n">
+        <v>57500.0</v>
+      </c>
+      <c r="C183" t="n">
+        <v>319900.0</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="n">
+        <v>1.01736E7</v>
+      </c>
+      <c r="B184" t="n">
+        <v>97500.0</v>
+      </c>
+      <c r="C184" t="n">
+        <v>313600.0</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="n">
+        <v>3.436956E8</v>
+      </c>
+      <c r="B185" t="n">
+        <v>106200.0</v>
+      </c>
+      <c r="C185" t="n">
+        <v>294200.0</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="n">
+        <v>4.6394E7</v>
+      </c>
+      <c r="B186" t="n">
+        <v>92300.0</v>
+      </c>
+      <c r="C186" t="n">
+        <v>360000.0</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="n">
+        <v>1.865883E8</v>
+      </c>
+      <c r="B187" t="n">
+        <v>97000.0</v>
+      </c>
+      <c r="C187" t="n">
+        <v>503400.0</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="n">
+        <v>2.766903E8</v>
+      </c>
+      <c r="B188" t="n">
+        <v>108800.0</v>
+      </c>
+      <c r="C188" t="n">
+        <v>325800.0</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="n">
+        <v>1.762053E8</v>
+      </c>
+      <c r="B189" t="n">
+        <v>190200.0</v>
+      </c>
+      <c r="C189" t="n">
+        <v>333800.0</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="n">
+        <v>4.352524E8</v>
+      </c>
+      <c r="B190" t="n">
+        <v>115200.0</v>
+      </c>
+      <c r="C190" t="n">
+        <v>392100.0</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="n">
+        <v>4.829238E8</v>
+      </c>
+      <c r="B191" t="n">
+        <v>180200.0</v>
+      </c>
+      <c r="C191" t="n">
+        <v>214900.0</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="n">
+        <v>4.806288E8</v>
+      </c>
+      <c r="B192" t="n">
+        <v>82700.0</v>
+      </c>
+      <c r="C192" t="n">
+        <v>202800.0</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="n">
+        <v>1.578296E8</v>
+      </c>
+      <c r="B193" t="n">
+        <v>99800.0</v>
+      </c>
+      <c r="C193" t="n">
+        <v>356200.0</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="n">
+        <v>1.491473E8</v>
+      </c>
+      <c r="B194" t="n">
+        <v>73900.0</v>
+      </c>
+      <c r="C194" t="n">
+        <v>334300.0</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="n">
+        <v>9.18425E7</v>
+      </c>
+      <c r="B195" t="n">
+        <v>76100.0</v>
+      </c>
+      <c r="C195" t="n">
+        <v>483500.0</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="n">
+        <v>4.709963E8</v>
+      </c>
+      <c r="B196" t="n">
+        <v>110300.0</v>
+      </c>
+      <c r="C196" t="n">
+        <v>213900.0</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="n">
+        <v>2.74847E8</v>
+      </c>
+      <c r="B197" t="n">
+        <v>159300.0</v>
+      </c>
+      <c r="C197" t="n">
+        <v>414100.0</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="n">
+        <v>2.329575E8</v>
+      </c>
+      <c r="B198" t="n">
+        <v>107500.0</v>
+      </c>
+      <c r="C198" t="n">
+        <v>631500.0</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="n">
+        <v>5.31852E7</v>
+      </c>
+      <c r="B199" t="n">
+        <v>76300.0</v>
+      </c>
+      <c r="C199" t="n">
+        <v>320100.0</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="n">
+        <v>4.91925E7</v>
+      </c>
+      <c r="B200" t="n">
+        <v>117000.0</v>
+      </c>
+      <c r="C200" t="n">
+        <v>308700.0</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="n">
+        <v>3.193298E8</v>
+      </c>
+      <c r="B201" t="n">
+        <v>100400.0</v>
+      </c>
+      <c r="C201" t="n">
+        <v>517300.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HeapSelect in O(n) + O(k log k)
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -513,1102 +513,1102 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>37700.0</v>
+        <v>3.51274599E10</v>
       </c>
       <c r="B2" t="n">
-        <v>447800.0</v>
+        <v>7488199.0</v>
       </c>
       <c r="C2" t="n">
-        <v>561000.0</v>
+        <v>1754300.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>17400.0</v>
+        <v>32501.0</v>
       </c>
       <c r="B3" t="n">
-        <v>4166.0</v>
+        <v>1599.0</v>
       </c>
       <c r="C3" t="n">
-        <v>10400.0</v>
+        <v>5100.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>11200.0</v>
+        <v>27300.0</v>
       </c>
       <c r="B4" t="n">
-        <v>4133.0</v>
+        <v>5850.0</v>
       </c>
       <c r="C4" t="n">
-        <v>7800.0</v>
+        <v>2650.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>12200.0</v>
+        <v>13300.0</v>
       </c>
       <c r="B5" t="n">
-        <v>16900.0</v>
+        <v>1916.0</v>
       </c>
       <c r="C5" t="n">
-        <v>51100.0</v>
+        <v>5450.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>17100.0</v>
+        <v>22800.0</v>
       </c>
       <c r="B6" t="n">
-        <v>3800.0</v>
+        <v>1733.0</v>
       </c>
       <c r="C6" t="n">
-        <v>11200.0</v>
+        <v>5100.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>11200.0</v>
+        <v>25899.0</v>
       </c>
       <c r="B7" t="n">
-        <v>3466.0</v>
+        <v>1900.0</v>
       </c>
       <c r="C7" t="n">
-        <v>6900.0</v>
+        <v>5249.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>10700.0</v>
+        <v>20200.0</v>
       </c>
       <c r="B8" t="n">
-        <v>15500.0</v>
+        <v>1750.0</v>
       </c>
       <c r="C8" t="n">
-        <v>21200.0</v>
+        <v>10201.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>37800.0</v>
+        <v>21500.0</v>
       </c>
       <c r="B9" t="n">
-        <v>4300.0</v>
+        <v>2099.0</v>
       </c>
       <c r="C9" t="n">
-        <v>10650.0</v>
+        <v>4033.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>11300.0</v>
+        <v>22000.0</v>
       </c>
       <c r="B10" t="n">
-        <v>5700.0</v>
+        <v>2900.0</v>
       </c>
       <c r="C10" t="n">
-        <v>6900.0</v>
+        <v>5649.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>12000.0</v>
+        <v>18601.0</v>
       </c>
       <c r="B11" t="n">
-        <v>4266.0</v>
+        <v>1766.0</v>
       </c>
       <c r="C11" t="n">
-        <v>6900.0</v>
+        <v>4067.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>33200.0</v>
+        <v>18200.0</v>
       </c>
       <c r="B12" t="n">
-        <v>16200.0</v>
+        <v>2080.0</v>
       </c>
       <c r="C12" t="n">
-        <v>8050.0</v>
+        <v>5850.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>14800.0</v>
+        <v>17999.0</v>
       </c>
       <c r="B13" t="n">
-        <v>12000.0</v>
+        <v>21099.0</v>
       </c>
       <c r="C13" t="n">
-        <v>12200.0</v>
+        <v>5550.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>17600.0</v>
+        <v>16200.0</v>
       </c>
       <c r="B14" t="n">
-        <v>621500.0</v>
+        <v>1571.0</v>
       </c>
       <c r="C14" t="n">
-        <v>47000.0</v>
+        <v>3699.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>19900.0</v>
+        <v>19200.0</v>
       </c>
       <c r="B15" t="n">
-        <v>12200.0</v>
+        <v>1599.0</v>
       </c>
       <c r="C15" t="n">
-        <v>14000.0</v>
+        <v>5549.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>10300.0</v>
+        <v>15800.0</v>
       </c>
       <c r="B16" t="n">
-        <v>3025.0</v>
+        <v>3766.0</v>
       </c>
       <c r="C16" t="n">
-        <v>5750.0</v>
+        <v>6600.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>8950.0</v>
+        <v>50301.0</v>
       </c>
       <c r="B17" t="n">
-        <v>24200.0</v>
+        <v>1885.0</v>
       </c>
       <c r="C17" t="n">
-        <v>12200.0</v>
+        <v>3799.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>14900.0</v>
+        <v>15100.0</v>
       </c>
       <c r="B18" t="n">
-        <v>3733.0</v>
+        <v>2000.0</v>
       </c>
       <c r="C18" t="n">
-        <v>8500.0</v>
+        <v>5300.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>9200.0</v>
+        <v>35001.0</v>
       </c>
       <c r="B19" t="n">
-        <v>4000.0</v>
+        <v>1300.0</v>
       </c>
       <c r="C19" t="n">
-        <v>12500.0</v>
+        <v>27999.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>10600.0</v>
+        <v>17301.0</v>
       </c>
       <c r="B20" t="n">
-        <v>4033.0</v>
+        <v>1866.0</v>
       </c>
       <c r="C20" t="n">
-        <v>6100.0</v>
+        <v>4433.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>9750.0</v>
+        <v>16600.0</v>
       </c>
       <c r="B21" t="n">
-        <v>4233.0</v>
+        <v>1733.0</v>
       </c>
       <c r="C21" t="n">
-        <v>6350.0</v>
+        <v>4166.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>10200.0</v>
+        <v>16500.0</v>
       </c>
       <c r="B22" t="n">
-        <v>3800.0</v>
+        <v>1499.0</v>
       </c>
       <c r="C22" t="n">
-        <v>5750.0</v>
+        <v>28900.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>14900.0</v>
+        <v>99601.0</v>
       </c>
       <c r="B23" t="n">
-        <v>5400.0</v>
+        <v>1700.0</v>
       </c>
       <c r="C23" t="n">
-        <v>5700.0</v>
+        <v>5100.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>10750.0</v>
+        <v>16999.0</v>
       </c>
       <c r="B24" t="n">
-        <v>2283.0</v>
+        <v>1571.0</v>
       </c>
       <c r="C24" t="n">
-        <v>14700.0</v>
+        <v>8200.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>24300.0</v>
+        <v>19401.0</v>
       </c>
       <c r="B25" t="n">
-        <v>12300.0</v>
+        <v>1816.0</v>
       </c>
       <c r="C25" t="n">
-        <v>16500.0</v>
+        <v>4133.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>17500.0</v>
+        <v>20000.0</v>
       </c>
       <c r="B26" t="n">
-        <v>1070.0</v>
+        <v>1683.0</v>
       </c>
       <c r="C26" t="n">
-        <v>18400.0</v>
+        <v>5900.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>15800.0</v>
+        <v>43200.0</v>
       </c>
       <c r="B27" t="n">
-        <v>1177.0</v>
+        <v>1866.0</v>
       </c>
       <c r="C27" t="n">
-        <v>18400.0</v>
+        <v>3900.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>17500.0</v>
+        <v>36199.0</v>
       </c>
       <c r="B28" t="n">
-        <v>1862.0</v>
+        <v>2383.0</v>
       </c>
       <c r="C28" t="n">
-        <v>16200.0</v>
+        <v>3600.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>11600.0</v>
+        <v>16300.0</v>
       </c>
       <c r="B29" t="n">
-        <v>650.0</v>
+        <v>1557.0</v>
       </c>
       <c r="C29" t="n">
-        <v>12900.0</v>
+        <v>5200.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>16700.0</v>
+        <v>20200.0</v>
       </c>
       <c r="B30" t="n">
-        <v>1060.0</v>
+        <v>10199.0</v>
       </c>
       <c r="C30" t="n">
-        <v>5650.0</v>
+        <v>3466.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>6500.0</v>
+        <v>11100.0</v>
       </c>
       <c r="B31" t="n">
-        <v>536.0</v>
+        <v>4100.0</v>
       </c>
       <c r="C31" t="n">
-        <v>5133.0</v>
+        <v>3433.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>11850.0</v>
+        <v>16600.0</v>
       </c>
       <c r="B32" t="n">
-        <v>403.0</v>
+        <v>1800.0</v>
       </c>
       <c r="C32" t="n">
-        <v>3866.0</v>
+        <v>3733.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>7550.0</v>
+        <v>30700.0</v>
       </c>
       <c r="B33" t="n">
-        <v>768033.0</v>
+        <v>6200.0</v>
       </c>
       <c r="C33" t="n">
-        <v>15500.0</v>
+        <v>1850.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>13400.0</v>
+        <v>25701.0</v>
       </c>
       <c r="B34" t="n">
-        <v>807.0</v>
+        <v>7500.0</v>
       </c>
       <c r="C34" t="n">
-        <v>15800.0</v>
+        <v>3866.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>19100.0</v>
+        <v>20500.0</v>
       </c>
       <c r="B35" t="n">
-        <v>643.0</v>
+        <v>1733.0</v>
       </c>
       <c r="C35" t="n">
-        <v>15000.0</v>
+        <v>8700.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>10100.0</v>
+        <v>10899.0</v>
       </c>
       <c r="B36" t="n">
-        <v>1400.0</v>
+        <v>900.0</v>
       </c>
       <c r="C36" t="n">
-        <v>7400.0</v>
+        <v>2200.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>9850.0</v>
+        <v>11099.0</v>
       </c>
       <c r="B37" t="n">
-        <v>807.0</v>
+        <v>927.0</v>
       </c>
       <c r="C37" t="n">
-        <v>19600.0</v>
+        <v>1799.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>30400.0</v>
+        <v>11600.0</v>
       </c>
       <c r="B38" t="n">
-        <v>686.0</v>
+        <v>1443.0</v>
       </c>
       <c r="C38" t="n">
-        <v>6850.0</v>
+        <v>2060.0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>6500.0</v>
+        <v>19000.0</v>
       </c>
       <c r="B39" t="n">
-        <v>728.0</v>
+        <v>6450.0</v>
       </c>
       <c r="C39" t="n">
-        <v>7150.0</v>
+        <v>2119.0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>10300.0</v>
+        <v>66200.0</v>
       </c>
       <c r="B40" t="n">
-        <v>1020.0</v>
+        <v>6274.0</v>
       </c>
       <c r="C40" t="n">
-        <v>6750.0</v>
+        <v>3833.0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>20400.0</v>
+        <v>19001.0</v>
       </c>
       <c r="B41" t="n">
-        <v>728.0</v>
+        <v>656.0</v>
       </c>
       <c r="C41" t="n">
-        <v>6000.0</v>
+        <v>3800.0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>16700.0</v>
+        <v>14600.0</v>
       </c>
       <c r="B42" t="n">
-        <v>757.0</v>
+        <v>5399.0</v>
       </c>
       <c r="C42" t="n">
-        <v>8300.0</v>
+        <v>7333.0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>10500.0</v>
+        <v>16800.0</v>
       </c>
       <c r="B43" t="n">
-        <v>726.0</v>
+        <v>351.0</v>
       </c>
       <c r="C43" t="n">
-        <v>6500.0</v>
+        <v>5450.0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>11100.0</v>
+        <v>17100.0</v>
       </c>
       <c r="B44" t="n">
-        <v>629.0</v>
+        <v>308.0</v>
       </c>
       <c r="C44" t="n">
-        <v>6150.0</v>
+        <v>3933.0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>12300.0</v>
+        <v>11800.0</v>
       </c>
       <c r="B45" t="n">
-        <v>700.0</v>
+        <v>2308120.0</v>
       </c>
       <c r="C45" t="n">
-        <v>13200.0</v>
+        <v>3699.0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>6000.0</v>
+        <v>13399.0</v>
       </c>
       <c r="B46" t="n">
-        <v>650.0</v>
+        <v>271.0</v>
       </c>
       <c r="C46" t="n">
-        <v>6100.0</v>
+        <v>3633.0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>6400.0</v>
+        <v>12600.0</v>
       </c>
       <c r="B47" t="n">
-        <v>858.0</v>
+        <v>283.0</v>
       </c>
       <c r="C47" t="n">
-        <v>6100.0</v>
+        <v>12500.0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>5950.0</v>
+        <v>12000.0</v>
       </c>
       <c r="B48" t="n">
-        <v>583.0</v>
+        <v>297.0</v>
       </c>
       <c r="C48" t="n">
-        <v>24400.0</v>
+        <v>10299.0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>8550.0</v>
+        <v>11999.0</v>
       </c>
       <c r="B49" t="n">
-        <v>757.0</v>
+        <v>229.0</v>
       </c>
       <c r="C49" t="n">
-        <v>5100.0</v>
+        <v>5750.0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>6800.0</v>
+        <v>6399.0</v>
       </c>
       <c r="B50" t="n">
-        <v>686.0</v>
+        <v>190.0</v>
       </c>
       <c r="C50" t="n">
-        <v>6650.0</v>
+        <v>12101.0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>13200.0</v>
+        <v>6450.0</v>
       </c>
       <c r="B51" t="n">
-        <v>662.0</v>
+        <v>364.0</v>
       </c>
       <c r="C51" t="n">
-        <v>8350.0</v>
+        <v>1020.0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>11100.0</v>
+        <v>5950.0</v>
       </c>
       <c r="B52" t="n">
-        <v>735.0</v>
+        <v>160.0</v>
       </c>
       <c r="C52" t="n">
-        <v>5350.0</v>
+        <v>1133.0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>6650.0</v>
+        <v>6550.0</v>
       </c>
       <c r="B53" t="n">
-        <v>1475.0</v>
+        <v>367.0</v>
       </c>
       <c r="C53" t="n">
-        <v>5100.0</v>
+        <v>2440.0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>6650.0</v>
+        <v>5949.0</v>
       </c>
       <c r="B54" t="n">
-        <v>686.0</v>
+        <v>159.0</v>
       </c>
       <c r="C54" t="n">
-        <v>5550.0</v>
+        <v>1000.0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>6550.0</v>
+        <v>5749.0</v>
       </c>
       <c r="B55" t="n">
-        <v>735.0</v>
+        <v>353.0</v>
       </c>
       <c r="C55" t="n">
-        <v>5550.0</v>
+        <v>963.0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>6200.0</v>
+        <v>18399.0</v>
       </c>
       <c r="B56" t="n">
-        <v>656.0</v>
+        <v>534.0</v>
       </c>
       <c r="C56" t="n">
-        <v>18300.0</v>
+        <v>5150.0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>6850.0</v>
+        <v>12400.0</v>
       </c>
       <c r="B57" t="n">
-        <v>1133.0</v>
+        <v>294.0</v>
       </c>
       <c r="C57" t="n">
-        <v>2100.0</v>
+        <v>1883.0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>6350.0</v>
+        <v>13000.0</v>
       </c>
       <c r="B58" t="n">
-        <v>713.0</v>
+        <v>400.0</v>
       </c>
       <c r="C58" t="n">
-        <v>2575.0</v>
+        <v>1766.0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>12100.0</v>
+        <v>12701.0</v>
       </c>
       <c r="B59" t="n">
-        <v>2550.0</v>
+        <v>305.0</v>
       </c>
       <c r="C59" t="n">
-        <v>3766.0</v>
+        <v>1337.0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>10200.0</v>
+        <v>14800.0</v>
       </c>
       <c r="B60" t="n">
-        <v>495.0</v>
+        <v>490.0</v>
       </c>
       <c r="C60" t="n">
-        <v>5300.0</v>
+        <v>1374.0</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>11600.0</v>
+        <v>13501.0</v>
       </c>
       <c r="B61" t="n">
-        <v>1030.0</v>
+        <v>329.0</v>
       </c>
       <c r="C61" t="n">
-        <v>5850.0</v>
+        <v>1166.0</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>10500.0</v>
+        <v>12700.0</v>
       </c>
       <c r="B62" t="n">
-        <v>160.0</v>
+        <v>302.0</v>
       </c>
       <c r="C62" t="n">
-        <v>1177.0</v>
+        <v>1049.0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>4000.0</v>
+        <v>12500.0</v>
       </c>
       <c r="B63" t="n">
-        <v>264.0</v>
+        <v>315.0</v>
       </c>
       <c r="C63" t="n">
-        <v>1040.0</v>
+        <v>1090.0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>6050.0</v>
+        <v>11700.0</v>
       </c>
       <c r="B64" t="n">
-        <v>152.0</v>
+        <v>283.0</v>
       </c>
       <c r="C64" t="n">
-        <v>1020.0</v>
+        <v>1040.0</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>3433.0</v>
+        <v>11799.0</v>
       </c>
       <c r="B65" t="n">
-        <v>152.0</v>
+        <v>300.0</v>
       </c>
       <c r="C65" t="n">
-        <v>1020.0</v>
+        <v>4450.0</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>5200.0</v>
+        <v>13299.0</v>
       </c>
       <c r="B66" t="n">
-        <v>2250.0</v>
+        <v>312.0</v>
       </c>
       <c r="C66" t="n">
-        <v>2233.0</v>
+        <v>1030.0</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>10700.0</v>
+        <v>61100.0</v>
       </c>
       <c r="B67" t="n">
-        <v>468.0</v>
+        <v>329.0</v>
       </c>
       <c r="C67" t="n">
-        <v>5600.0</v>
+        <v>1287.0</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>5550.0</v>
+        <v>13200.0</v>
       </c>
       <c r="B68" t="n">
-        <v>445.0</v>
+        <v>447.0</v>
       </c>
       <c r="C68" t="n">
-        <v>5200.0</v>
+        <v>1716.0</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>6000.0</v>
+        <v>28900.0</v>
       </c>
       <c r="B69" t="n">
-        <v>214.0</v>
+        <v>294.0</v>
       </c>
       <c r="C69" t="n">
-        <v>2675.0</v>
+        <v>1110.0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>5700.0</v>
+        <v>28101.0</v>
       </c>
       <c r="B70" t="n">
-        <v>214.0</v>
+        <v>309.0</v>
       </c>
       <c r="C70" t="n">
-        <v>2320.0</v>
+        <v>1059.0</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>6650.0</v>
+        <v>10899.0</v>
       </c>
       <c r="B71" t="n">
-        <v>408.0</v>
+        <v>360.0</v>
       </c>
       <c r="C71" t="n">
-        <v>2160.0</v>
+        <v>1059.0</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>7700.0</v>
+        <v>13400.0</v>
       </c>
       <c r="B72" t="n">
-        <v>288.0</v>
+        <v>265.0</v>
       </c>
       <c r="C72" t="n">
-        <v>2650.0</v>
+        <v>963.0</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>7200.0</v>
+        <v>8100.0</v>
       </c>
       <c r="B73" t="n">
-        <v>315.0</v>
+        <v>286.0</v>
       </c>
       <c r="C73" t="n">
-        <v>2700.0</v>
+        <v>1716.0</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>6300.0</v>
+        <v>7800.0</v>
       </c>
       <c r="B74" t="n">
-        <v>261.0</v>
+        <v>2058.0</v>
       </c>
       <c r="C74" t="n">
-        <v>2060.0</v>
+        <v>954.0</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>11300.0</v>
+        <v>12000.0</v>
       </c>
       <c r="B75" t="n">
-        <v>408.0</v>
+        <v>259.0</v>
       </c>
       <c r="C75" t="n">
-        <v>2700.0</v>
+        <v>1144.0</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>6000.0</v>
+        <v>11300.0</v>
       </c>
       <c r="B76" t="n">
-        <v>412.0</v>
+        <v>351.0</v>
       </c>
       <c r="C76" t="n">
-        <v>5750.0</v>
+        <v>1020.0</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>6950.0</v>
+        <v>10300.0</v>
       </c>
       <c r="B77" t="n">
-        <v>245.0</v>
+        <v>281.0</v>
       </c>
       <c r="C77" t="n">
-        <v>2550.0</v>
+        <v>700.0</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>5700.0</v>
+        <v>5600.0</v>
       </c>
       <c r="B78" t="n">
-        <v>221.0</v>
+        <v>336.0</v>
       </c>
       <c r="C78" t="n">
-        <v>2675.0</v>
+        <v>600.0</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>6350.0</v>
+        <v>5099.0</v>
       </c>
       <c r="B79" t="n">
-        <v>332.0</v>
+        <v>192.0</v>
       </c>
       <c r="C79" t="n">
-        <v>2300.0</v>
+        <v>1059.0</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>5550.0</v>
+        <v>7300.0</v>
       </c>
       <c r="B80" t="n">
-        <v>217.0</v>
+        <v>542.0</v>
       </c>
       <c r="C80" t="n">
-        <v>1883.0</v>
+        <v>572.0</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>6150.0</v>
+        <v>5500.0</v>
       </c>
       <c r="B81" t="n">
-        <v>261.0</v>
+        <v>194.0</v>
       </c>
       <c r="C81" t="n">
-        <v>2160.0</v>
+        <v>1155.0</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>6300.0</v>
+        <v>7300.0</v>
       </c>
       <c r="B82" t="n">
-        <v>247.0</v>
+        <v>156.0</v>
       </c>
       <c r="C82" t="n">
-        <v>7750.0</v>
+        <v>510.0</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>7600.0</v>
+        <v>5250.0</v>
       </c>
       <c r="B83" t="n">
-        <v>907.0</v>
+        <v>158.0</v>
       </c>
       <c r="C83" t="n">
-        <v>2600.0</v>
+        <v>520.0</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>8850.0</v>
+        <v>4500.0</v>
       </c>
       <c r="B84" t="n">
-        <v>264.0</v>
+        <v>156.0</v>
       </c>
       <c r="C84" t="n">
-        <v>2825.0</v>
+        <v>510.0</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>6750.0</v>
+        <v>18099.0</v>
       </c>
       <c r="B85" t="n">
-        <v>294.0</v>
+        <v>477.0</v>
       </c>
       <c r="C85" t="n">
-        <v>5400.0</v>
+        <v>271.0</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>6200.0</v>
+        <v>11001.0</v>
       </c>
       <c r="B86" t="n">
-        <v>248.0</v>
+        <v>318.0</v>
       </c>
       <c r="C86" t="n">
-        <v>891.0</v>
+        <v>443.0</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>5800.0</v>
+        <v>10700.0</v>
       </c>
       <c r="B87" t="n">
-        <v>403.0</v>
+        <v>312.0</v>
       </c>
       <c r="C87" t="n">
-        <v>927.0</v>
+        <v>552.0</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>6600.0</v>
+        <v>25200.0</v>
       </c>
       <c r="B88" t="n">
-        <v>1040.0</v>
+        <v>420.0</v>
       </c>
       <c r="C88" t="n">
-        <v>875.0</v>
+        <v>536.0</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>6500.0</v>
+        <v>10499.0</v>
       </c>
       <c r="B89" t="n">
-        <v>231.0</v>
+        <v>261.0</v>
       </c>
       <c r="C89" t="n">
-        <v>883.0</v>
+        <v>519.0</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>5500.0</v>
+        <v>6449.0</v>
       </c>
       <c r="B90" t="n">
-        <v>212.0</v>
+        <v>161.0</v>
       </c>
       <c r="C90" t="n">
-        <v>875.0</v>
+        <v>728.0</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>5150.0</v>
+        <v>8300.0</v>
       </c>
       <c r="B91" t="n">
-        <v>206.0</v>
+        <v>242.0</v>
       </c>
       <c r="C91" t="n">
-        <v>1188.0</v>
+        <v>536.0</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>6550.0</v>
+        <v>5199.0</v>
       </c>
       <c r="B92" t="n">
-        <v>212.0</v>
+        <v>583.0</v>
       </c>
       <c r="C92" t="n">
-        <v>945.0</v>
+        <v>275.0</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>10050.0</v>
+        <v>10300.0</v>
       </c>
       <c r="B93" t="n">
-        <v>187.0</v>
+        <v>200.0</v>
       </c>
       <c r="C93" t="n">
-        <v>858.0</v>
+        <v>271.0</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>5550.0</v>
+        <v>15100.0</v>
       </c>
       <c r="B94" t="n">
-        <v>192.0</v>
+        <v>190.0</v>
       </c>
       <c r="C94" t="n">
-        <v>916.0</v>
+        <v>273.0</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>7300.0</v>
+        <v>4166.0</v>
       </c>
       <c r="B95" t="n">
-        <v>206.0</v>
+        <v>180.0</v>
       </c>
       <c r="C95" t="n">
-        <v>1040.0</v>
+        <v>268.0</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>6300.0</v>
+        <v>4133.0</v>
       </c>
       <c r="B96" t="n">
-        <v>216.0</v>
+        <v>1161.0</v>
       </c>
       <c r="C96" t="n">
-        <v>936.0</v>
+        <v>374.0</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>12100.0</v>
+        <v>4199.0</v>
       </c>
       <c r="B97" t="n">
-        <v>217.0</v>
+        <v>271.0</v>
       </c>
       <c r="C97" t="n">
-        <v>936.0</v>
+        <v>460.0</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>5750.0</v>
+        <v>7349.0</v>
       </c>
       <c r="B98" t="n">
-        <v>201.0</v>
+        <v>278.0</v>
       </c>
       <c r="C98" t="n">
-        <v>1300.0</v>
+        <v>377.0</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>10600.0</v>
+        <v>11001.0</v>
       </c>
       <c r="B99" t="n">
-        <v>365.0</v>
+        <v>306.0</v>
       </c>
       <c r="C99" t="n">
-        <v>1133.0</v>
+        <v>536.0</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>7200.0</v>
+        <v>4200.0</v>
       </c>
       <c r="B100" t="n">
-        <v>504.0</v>
+        <v>429.0</v>
       </c>
       <c r="C100" t="n">
-        <v>1211.0</v>
+        <v>815.0</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>8550.0</v>
+        <v>16800.0</v>
       </c>
       <c r="B101" t="n">
-        <v>520.0</v>
+        <v>201.0</v>
       </c>
       <c r="C101" t="n">
-        <v>1020.0</v>
+        <v>283.0</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
HeapSelect O(k log k)
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -513,1102 +513,1102 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>3.51274599E10</v>
+        <v>2000.0</v>
       </c>
       <c r="B2" t="n">
-        <v>7488199.0</v>
+        <v>585400.0</v>
       </c>
       <c r="C2" t="n">
-        <v>1754300.0</v>
+        <v>556400.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>32501.0</v>
+        <v>823.0</v>
       </c>
       <c r="B3" t="n">
-        <v>1599.0</v>
+        <v>5500.0</v>
       </c>
       <c r="C3" t="n">
-        <v>5100.0</v>
+        <v>7300.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>27300.0</v>
+        <v>750.0</v>
       </c>
       <c r="B4" t="n">
-        <v>5850.0</v>
+        <v>2800.0</v>
       </c>
       <c r="C4" t="n">
-        <v>2650.0</v>
+        <v>5400.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>13300.0</v>
+        <v>1571.0</v>
       </c>
       <c r="B5" t="n">
-        <v>1916.0</v>
+        <v>2825.0</v>
       </c>
       <c r="C5" t="n">
-        <v>5450.0</v>
+        <v>5750.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>22800.0</v>
+        <v>412.0</v>
       </c>
       <c r="B6" t="n">
-        <v>1733.0</v>
+        <v>11400.0</v>
       </c>
       <c r="C6" t="n">
-        <v>5100.0</v>
+        <v>21700.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>25899.0</v>
+        <v>385.0</v>
       </c>
       <c r="B7" t="n">
-        <v>1900.0</v>
+        <v>3000.0</v>
       </c>
       <c r="C7" t="n">
-        <v>5249.0</v>
+        <v>5100.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>20200.0</v>
+        <v>1027.0</v>
       </c>
       <c r="B8" t="n">
-        <v>1750.0</v>
+        <v>11600.0</v>
       </c>
       <c r="C8" t="n">
-        <v>10201.0</v>
+        <v>13700.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>21500.0</v>
+        <v>750.0</v>
       </c>
       <c r="B9" t="n">
-        <v>2099.0</v>
+        <v>2675.0</v>
       </c>
       <c r="C9" t="n">
-        <v>4033.0</v>
+        <v>4366.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>22000.0</v>
+        <v>792.0</v>
       </c>
       <c r="B10" t="n">
-        <v>2900.0</v>
+        <v>11500.0</v>
       </c>
       <c r="C10" t="n">
-        <v>5649.0</v>
+        <v>10050.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>18601.0</v>
+        <v>385.0</v>
       </c>
       <c r="B11" t="n">
-        <v>1766.0</v>
+        <v>2700.0</v>
       </c>
       <c r="C11" t="n">
-        <v>4067.0</v>
+        <v>5200.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>18200.0</v>
+        <v>392.0</v>
       </c>
       <c r="B12" t="n">
-        <v>2080.0</v>
+        <v>3466.0</v>
       </c>
       <c r="C12" t="n">
-        <v>5850.0</v>
+        <v>5700.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>17999.0</v>
+        <v>318.0</v>
       </c>
       <c r="B13" t="n">
-        <v>21099.0</v>
+        <v>2725.0</v>
       </c>
       <c r="C13" t="n">
-        <v>5550.0</v>
+        <v>3733.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>16200.0</v>
+        <v>815.0</v>
       </c>
       <c r="B14" t="n">
-        <v>1571.0</v>
+        <v>11200.0</v>
       </c>
       <c r="C14" t="n">
-        <v>3699.0</v>
+        <v>9100.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>19200.0</v>
+        <v>1900.0</v>
       </c>
       <c r="B15" t="n">
-        <v>1599.0</v>
+        <v>2725.0</v>
       </c>
       <c r="C15" t="n">
-        <v>5549.0</v>
+        <v>10800.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>15800.0</v>
+        <v>680.0</v>
       </c>
       <c r="B16" t="n">
-        <v>3766.0</v>
+        <v>5250.0</v>
       </c>
       <c r="C16" t="n">
-        <v>6600.0</v>
+        <v>6150.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>50301.0</v>
+        <v>623.0</v>
       </c>
       <c r="B17" t="n">
-        <v>1885.0</v>
+        <v>5400.0</v>
       </c>
       <c r="C17" t="n">
-        <v>3799.0</v>
+        <v>5850.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>15100.0</v>
+        <v>542.0</v>
       </c>
       <c r="B18" t="n">
-        <v>2000.0</v>
+        <v>7233.0</v>
       </c>
       <c r="C18" t="n">
-        <v>5300.0</v>
+        <v>6000.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>35001.0</v>
+        <v>1300.0</v>
       </c>
       <c r="B19" t="n">
-        <v>1300.0</v>
+        <v>4600.0</v>
       </c>
       <c r="C19" t="n">
-        <v>27999.0</v>
+        <v>6100.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>17301.0</v>
+        <v>1168.0</v>
       </c>
       <c r="B20" t="n">
-        <v>1866.0</v>
+        <v>5350.0</v>
       </c>
       <c r="C20" t="n">
-        <v>4433.0</v>
+        <v>6100.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>16600.0</v>
+        <v>4774950.0</v>
       </c>
       <c r="B21" t="n">
-        <v>1733.0</v>
+        <v>11700.0</v>
       </c>
       <c r="C21" t="n">
-        <v>4166.0</v>
+        <v>6550.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>16500.0</v>
+        <v>1636.0</v>
       </c>
       <c r="B22" t="n">
-        <v>1499.0</v>
+        <v>5400.0</v>
       </c>
       <c r="C22" t="n">
-        <v>28900.0</v>
+        <v>6150.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>99601.0</v>
+        <v>385.0</v>
       </c>
       <c r="B23" t="n">
-        <v>1700.0</v>
+        <v>8466.0</v>
       </c>
       <c r="C23" t="n">
-        <v>5100.0</v>
+        <v>6300.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>16999.0</v>
+        <v>412.0</v>
       </c>
       <c r="B24" t="n">
-        <v>1571.0</v>
+        <v>7500.0</v>
       </c>
       <c r="C24" t="n">
-        <v>8200.0</v>
+        <v>10200.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>19401.0</v>
+        <v>364.0</v>
       </c>
       <c r="B25" t="n">
-        <v>1816.0</v>
+        <v>3400.0</v>
       </c>
       <c r="C25" t="n">
-        <v>4133.0</v>
+        <v>7650.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>20000.0</v>
+        <v>452.0</v>
       </c>
       <c r="B26" t="n">
-        <v>1683.0</v>
+        <v>706.0</v>
       </c>
       <c r="C26" t="n">
-        <v>5900.0</v>
+        <v>13100.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>43200.0</v>
+        <v>346.0</v>
       </c>
       <c r="B27" t="n">
-        <v>1866.0</v>
+        <v>742.0</v>
       </c>
       <c r="C27" t="n">
-        <v>3900.0</v>
+        <v>14850.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>36199.0</v>
+        <v>945.0</v>
       </c>
       <c r="B28" t="n">
-        <v>2383.0</v>
+        <v>784.0</v>
       </c>
       <c r="C28" t="n">
-        <v>3600.0</v>
+        <v>6250.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>16300.0</v>
+        <v>412.0</v>
       </c>
       <c r="B29" t="n">
-        <v>1557.0</v>
+        <v>675.0</v>
       </c>
       <c r="C29" t="n">
-        <v>5200.0</v>
+        <v>6900.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>20200.0</v>
+        <v>3044.0</v>
       </c>
       <c r="B30" t="n">
-        <v>10199.0</v>
+        <v>785.0</v>
       </c>
       <c r="C30" t="n">
-        <v>3466.0</v>
+        <v>10400.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>11100.0</v>
+        <v>355.0</v>
       </c>
       <c r="B31" t="n">
-        <v>4100.0</v>
+        <v>680.0</v>
       </c>
       <c r="C31" t="n">
-        <v>3433.0</v>
+        <v>6700.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>16600.0</v>
+        <v>375.0</v>
       </c>
       <c r="B32" t="n">
-        <v>1800.0</v>
+        <v>981.0</v>
       </c>
       <c r="C32" t="n">
-        <v>3733.0</v>
+        <v>6000.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>30700.0</v>
+        <v>400.0</v>
       </c>
       <c r="B33" t="n">
-        <v>6200.0</v>
+        <v>866.0</v>
       </c>
       <c r="C33" t="n">
-        <v>1850.0</v>
+        <v>13400.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>25701.0</v>
+        <v>358.0</v>
       </c>
       <c r="B34" t="n">
-        <v>7500.0</v>
+        <v>568.0</v>
       </c>
       <c r="C34" t="n">
-        <v>3866.0</v>
+        <v>8100.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>20500.0</v>
+        <v>9650.0</v>
       </c>
       <c r="B35" t="n">
-        <v>1733.0</v>
+        <v>617.0</v>
       </c>
       <c r="C35" t="n">
-        <v>8700.0</v>
+        <v>6400.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>10899.0</v>
+        <v>778.0</v>
       </c>
       <c r="B36" t="n">
-        <v>900.0</v>
+        <v>600.0</v>
       </c>
       <c r="C36" t="n">
-        <v>2200.0</v>
+        <v>26200.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>11099.0</v>
+        <v>392.0</v>
       </c>
       <c r="B37" t="n">
-        <v>927.0</v>
+        <v>800.0</v>
       </c>
       <c r="C37" t="n">
-        <v>1799.0</v>
+        <v>6400.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>11600.0</v>
+        <v>2000.0</v>
       </c>
       <c r="B38" t="n">
-        <v>1443.0</v>
+        <v>588.0</v>
       </c>
       <c r="C38" t="n">
-        <v>2060.0</v>
+        <v>10200.0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>19000.0</v>
+        <v>278.0</v>
       </c>
       <c r="B39" t="n">
-        <v>6450.0</v>
+        <v>792.0</v>
       </c>
       <c r="C39" t="n">
-        <v>2119.0</v>
+        <v>5500.0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>66200.0</v>
+        <v>1097.0</v>
       </c>
       <c r="B40" t="n">
-        <v>6274.0</v>
+        <v>547.0</v>
       </c>
       <c r="C40" t="n">
-        <v>3833.0</v>
+        <v>7650.0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>19001.0</v>
+        <v>166.0</v>
       </c>
       <c r="B41" t="n">
-        <v>656.0</v>
+        <v>662.0</v>
       </c>
       <c r="C41" t="n">
-        <v>3800.0</v>
+        <v>11200.0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>14600.0</v>
+        <v>468.0</v>
       </c>
       <c r="B42" t="n">
-        <v>5399.0</v>
+        <v>611.0</v>
       </c>
       <c r="C42" t="n">
-        <v>7333.0</v>
+        <v>10600.0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>16800.0</v>
+        <v>396.0</v>
       </c>
       <c r="B43" t="n">
-        <v>351.0</v>
+        <v>656.0</v>
       </c>
       <c r="C43" t="n">
-        <v>5450.0</v>
+        <v>11950.0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>17100.0</v>
+        <v>351.0</v>
       </c>
       <c r="B44" t="n">
-        <v>308.0</v>
+        <v>600.0</v>
       </c>
       <c r="C44" t="n">
-        <v>3933.0</v>
+        <v>5850.0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>11800.0</v>
+        <v>206.0</v>
       </c>
       <c r="B45" t="n">
-        <v>2308120.0</v>
+        <v>784.0</v>
       </c>
       <c r="C45" t="n">
-        <v>3699.0</v>
+        <v>10600.0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>13399.0</v>
+        <v>177.0</v>
       </c>
       <c r="B46" t="n">
-        <v>271.0</v>
+        <v>771.0</v>
       </c>
       <c r="C46" t="n">
-        <v>3633.0</v>
+        <v>6400.0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>12600.0</v>
+        <v>198.0</v>
       </c>
       <c r="B47" t="n">
-        <v>283.0</v>
+        <v>2200.0</v>
       </c>
       <c r="C47" t="n">
-        <v>12500.0</v>
+        <v>6450.0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>12000.0</v>
+        <v>194.0</v>
       </c>
       <c r="B48" t="n">
-        <v>297.0</v>
+        <v>1163.0</v>
       </c>
       <c r="C48" t="n">
-        <v>10299.0</v>
+        <v>17800.0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>11999.0</v>
+        <v>231.0</v>
       </c>
       <c r="B49" t="n">
-        <v>229.0</v>
+        <v>958.0</v>
       </c>
       <c r="C49" t="n">
-        <v>5750.0</v>
+        <v>8500.0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>6399.0</v>
+        <v>245.0</v>
       </c>
       <c r="B50" t="n">
-        <v>190.0</v>
+        <v>605.0</v>
       </c>
       <c r="C50" t="n">
-        <v>12101.0</v>
+        <v>6000.0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>6450.0</v>
+        <v>204.0</v>
       </c>
       <c r="B51" t="n">
-        <v>364.0</v>
+        <v>706.0</v>
       </c>
       <c r="C51" t="n">
-        <v>1020.0</v>
+        <v>6400.0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>5950.0</v>
+        <v>214.0</v>
       </c>
       <c r="B52" t="n">
-        <v>160.0</v>
+        <v>568.0</v>
       </c>
       <c r="C52" t="n">
-        <v>1133.0</v>
+        <v>5650.0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>6550.0</v>
+        <v>187.0</v>
       </c>
       <c r="B53" t="n">
-        <v>367.0</v>
+        <v>750.0</v>
       </c>
       <c r="C53" t="n">
-        <v>2440.0</v>
+        <v>8200.0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>5949.0</v>
+        <v>226.0</v>
       </c>
       <c r="B54" t="n">
-        <v>159.0</v>
+        <v>1275.0</v>
       </c>
       <c r="C54" t="n">
-        <v>1000.0</v>
+        <v>31050.0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>5749.0</v>
+        <v>231.0</v>
       </c>
       <c r="B55" t="n">
-        <v>353.0</v>
+        <v>757.0</v>
       </c>
       <c r="C55" t="n">
-        <v>963.0</v>
+        <v>5100.0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>18399.0</v>
+        <v>210.0</v>
       </c>
       <c r="B56" t="n">
-        <v>534.0</v>
+        <v>1155.0</v>
       </c>
       <c r="C56" t="n">
-        <v>5150.0</v>
+        <v>18800.0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>12400.0</v>
+        <v>230.0</v>
       </c>
       <c r="B57" t="n">
-        <v>294.0</v>
+        <v>680.0</v>
       </c>
       <c r="C57" t="n">
-        <v>1883.0</v>
+        <v>1783.0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>13000.0</v>
+        <v>192.0</v>
       </c>
       <c r="B58" t="n">
-        <v>400.0</v>
+        <v>3400.0</v>
       </c>
       <c r="C58" t="n">
-        <v>1766.0</v>
+        <v>2100.0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>12701.0</v>
+        <v>214.0</v>
       </c>
       <c r="B59" t="n">
-        <v>305.0</v>
+        <v>311.0</v>
       </c>
       <c r="C59" t="n">
-        <v>1337.0</v>
+        <v>4033.0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>14800.0</v>
+        <v>196.0</v>
       </c>
       <c r="B60" t="n">
-        <v>490.0</v>
+        <v>300.0</v>
       </c>
       <c r="C60" t="n">
-        <v>1374.0</v>
+        <v>1866.0</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>13501.0</v>
+        <v>223.0</v>
       </c>
       <c r="B61" t="n">
-        <v>329.0</v>
+        <v>364.0</v>
       </c>
       <c r="C61" t="n">
-        <v>1166.0</v>
+        <v>2625.0</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>12700.0</v>
+        <v>196.0</v>
       </c>
       <c r="B62" t="n">
-        <v>302.0</v>
+        <v>367.0</v>
       </c>
       <c r="C62" t="n">
-        <v>1049.0</v>
+        <v>2280.0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>12500.0</v>
+        <v>192.0</v>
       </c>
       <c r="B63" t="n">
-        <v>315.0</v>
+        <v>328.0</v>
       </c>
       <c r="C63" t="n">
-        <v>1090.0</v>
+        <v>2100.0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>11700.0</v>
+        <v>183.0</v>
       </c>
       <c r="B64" t="n">
-        <v>283.0</v>
+        <v>321.0</v>
       </c>
       <c r="C64" t="n">
-        <v>1040.0</v>
+        <v>2100.0</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>11799.0</v>
+        <v>174.0</v>
       </c>
       <c r="B65" t="n">
-        <v>300.0</v>
+        <v>500.0</v>
       </c>
       <c r="C65" t="n">
-        <v>4450.0</v>
+        <v>2180.0</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>13299.0</v>
+        <v>256.0</v>
       </c>
       <c r="B66" t="n">
-        <v>312.0</v>
+        <v>351.0</v>
       </c>
       <c r="C66" t="n">
-        <v>1030.0</v>
+        <v>2800.0</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>61100.0</v>
+        <v>275.0</v>
       </c>
       <c r="B67" t="n">
-        <v>329.0</v>
+        <v>355.0</v>
       </c>
       <c r="C67" t="n">
-        <v>1287.0</v>
+        <v>3150.0</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>13200.0</v>
+        <v>174.0</v>
       </c>
       <c r="B68" t="n">
-        <v>447.0</v>
+        <v>288.0</v>
       </c>
       <c r="C68" t="n">
-        <v>1716.0</v>
+        <v>1966.0</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>28900.0</v>
+        <v>196.0</v>
       </c>
       <c r="B69" t="n">
-        <v>294.0</v>
+        <v>477.0</v>
       </c>
       <c r="C69" t="n">
-        <v>1110.0</v>
+        <v>3633.0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>28101.0</v>
+        <v>242.0</v>
       </c>
       <c r="B70" t="n">
-        <v>309.0</v>
+        <v>308.0</v>
       </c>
       <c r="C70" t="n">
-        <v>1059.0</v>
+        <v>3120.0</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>10899.0</v>
+        <v>210.0</v>
       </c>
       <c r="B71" t="n">
-        <v>360.0</v>
+        <v>335.0</v>
       </c>
       <c r="C71" t="n">
-        <v>1059.0</v>
+        <v>2260.0</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>13400.0</v>
+        <v>212.0</v>
       </c>
       <c r="B72" t="n">
-        <v>265.0</v>
+        <v>221.0</v>
       </c>
       <c r="C72" t="n">
-        <v>963.0</v>
+        <v>1155.0</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>8100.0</v>
+        <v>114.0</v>
       </c>
       <c r="B73" t="n">
-        <v>286.0</v>
+        <v>185.0</v>
       </c>
       <c r="C73" t="n">
-        <v>1716.0</v>
+        <v>1030.0</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>7800.0</v>
+        <v>152.0</v>
       </c>
       <c r="B74" t="n">
-        <v>2058.0</v>
+        <v>623.0</v>
       </c>
       <c r="C74" t="n">
-        <v>954.0</v>
+        <v>2750.0</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>12000.0</v>
+        <v>245.0</v>
       </c>
       <c r="B75" t="n">
-        <v>259.0</v>
+        <v>332.0</v>
       </c>
       <c r="C75" t="n">
-        <v>1144.0</v>
+        <v>2200.0</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>11300.0</v>
+        <v>210.0</v>
       </c>
       <c r="B76" t="n">
-        <v>351.0</v>
+        <v>408.0</v>
       </c>
       <c r="C76" t="n">
-        <v>1020.0</v>
+        <v>2200.0</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>10300.0</v>
+        <v>294.0</v>
       </c>
       <c r="B77" t="n">
-        <v>281.0</v>
+        <v>510.0</v>
       </c>
       <c r="C77" t="n">
-        <v>700.0</v>
+        <v>2380.0</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>5600.0</v>
+        <v>188.0</v>
       </c>
       <c r="B78" t="n">
-        <v>336.0</v>
+        <v>271.0</v>
       </c>
       <c r="C78" t="n">
-        <v>600.0</v>
+        <v>2080.0</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>5099.0</v>
+        <v>210.0</v>
       </c>
       <c r="B79" t="n">
-        <v>192.0</v>
+        <v>385.0</v>
       </c>
       <c r="C79" t="n">
-        <v>1059.0</v>
+        <v>2040.0</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>7300.0</v>
+        <v>170.0</v>
       </c>
       <c r="B80" t="n">
-        <v>542.0</v>
+        <v>245.0</v>
       </c>
       <c r="C80" t="n">
-        <v>572.0</v>
+        <v>2700.0</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>5500.0</v>
+        <v>118.0</v>
       </c>
       <c r="B81" t="n">
-        <v>194.0</v>
+        <v>176.0</v>
       </c>
       <c r="C81" t="n">
-        <v>1155.0</v>
+        <v>1733.0</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>7300.0</v>
+        <v>110.0</v>
       </c>
       <c r="B82" t="n">
-        <v>156.0</v>
+        <v>515.0</v>
       </c>
       <c r="C82" t="n">
-        <v>510.0</v>
+        <v>6850.0</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>5250.0</v>
+        <v>117.0</v>
       </c>
       <c r="B83" t="n">
-        <v>158.0</v>
+        <v>219.0</v>
       </c>
       <c r="C83" t="n">
-        <v>520.0</v>
+        <v>1275.0</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>4500.0</v>
+        <v>114.0</v>
       </c>
       <c r="B84" t="n">
-        <v>156.0</v>
+        <v>174.0</v>
       </c>
       <c r="C84" t="n">
-        <v>510.0</v>
+        <v>735.0</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>18099.0</v>
+        <v>112.0</v>
       </c>
       <c r="B85" t="n">
-        <v>477.0</v>
+        <v>208.0</v>
       </c>
       <c r="C85" t="n">
-        <v>271.0</v>
+        <v>500.0</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>11001.0</v>
+        <v>113.0</v>
       </c>
       <c r="B86" t="n">
-        <v>318.0</v>
+        <v>343.0</v>
       </c>
       <c r="C86" t="n">
-        <v>443.0</v>
+        <v>500.0</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>10700.0</v>
+        <v>204.0</v>
       </c>
       <c r="B87" t="n">
-        <v>312.0</v>
+        <v>358.0</v>
       </c>
       <c r="C87" t="n">
-        <v>552.0</v>
+        <v>1471.0</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>25200.0</v>
+        <v>214.0</v>
       </c>
       <c r="B88" t="n">
-        <v>420.0</v>
+        <v>425.0</v>
       </c>
       <c r="C88" t="n">
-        <v>536.0</v>
+        <v>936.0</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>10499.0</v>
+        <v>201.0</v>
       </c>
       <c r="B89" t="n">
-        <v>261.0</v>
+        <v>329.0</v>
       </c>
       <c r="C89" t="n">
-        <v>519.0</v>
+        <v>900.0</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>6449.0</v>
+        <v>182.0</v>
       </c>
       <c r="B90" t="n">
-        <v>161.0</v>
+        <v>350.0</v>
       </c>
       <c r="C90" t="n">
-        <v>728.0</v>
+        <v>990.0</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>8300.0</v>
+        <v>118.0</v>
       </c>
       <c r="B91" t="n">
-        <v>242.0</v>
+        <v>214.0</v>
       </c>
       <c r="C91" t="n">
-        <v>536.0</v>
+        <v>510.0</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>5199.0</v>
+        <v>143.0</v>
       </c>
       <c r="B92" t="n">
-        <v>583.0</v>
+        <v>178.0</v>
       </c>
       <c r="C92" t="n">
-        <v>275.0</v>
+        <v>566.0</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>10300.0</v>
+        <v>217.0</v>
       </c>
       <c r="B93" t="n">
-        <v>200.0</v>
+        <v>1700.0</v>
       </c>
       <c r="C93" t="n">
-        <v>271.0</v>
+        <v>936.0</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>15100.0</v>
+        <v>210.0</v>
       </c>
       <c r="B94" t="n">
-        <v>190.0</v>
+        <v>201.0</v>
       </c>
       <c r="C94" t="n">
-        <v>273.0</v>
+        <v>963.0</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>4166.0</v>
+        <v>206.0</v>
       </c>
       <c r="B95" t="n">
-        <v>180.0</v>
+        <v>245.0</v>
       </c>
       <c r="C95" t="n">
-        <v>268.0</v>
+        <v>972.0</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>4133.0</v>
+        <v>429.0</v>
       </c>
       <c r="B96" t="n">
-        <v>1161.0</v>
+        <v>237.0</v>
       </c>
       <c r="C96" t="n">
-        <v>374.0</v>
+        <v>1009.0</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>4199.0</v>
+        <v>196.0</v>
       </c>
       <c r="B97" t="n">
-        <v>271.0</v>
+        <v>212.0</v>
       </c>
       <c r="C97" t="n">
-        <v>460.0</v>
+        <v>945.0</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>7349.0</v>
+        <v>212.0</v>
       </c>
       <c r="B98" t="n">
-        <v>278.0</v>
+        <v>247.0</v>
       </c>
       <c r="C98" t="n">
-        <v>377.0</v>
+        <v>2540.0</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>11001.0</v>
+        <v>196.0</v>
       </c>
       <c r="B99" t="n">
-        <v>306.0</v>
+        <v>247.0</v>
       </c>
       <c r="C99" t="n">
-        <v>536.0</v>
+        <v>954.0</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>4200.0</v>
+        <v>201.0</v>
       </c>
       <c r="B100" t="n">
-        <v>429.0</v>
+        <v>245.0</v>
       </c>
       <c r="C100" t="n">
-        <v>815.0</v>
+        <v>981.0</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>16800.0</v>
+        <v>258.0</v>
       </c>
       <c r="B101" t="n">
-        <v>201.0</v>
+        <v>236.0</v>
       </c>
       <c r="C101" t="n">
-        <v>283.0</v>
+        <v>866.0</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>